<commit_message>
Add BaseBall items (1,2,3,PlayerLoad)
</commit_message>
<xml_diff>
--- a/Web/WebLocalization.xlsx
+++ b/Web/WebLocalization.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4080" uniqueCount="3215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4095" uniqueCount="3224">
   <si>
     <t>key</t>
   </si>
@@ -16039,6 +16039,33 @@
   </si>
   <si>
     <t>Base Ball Score High</t>
+  </si>
+  <si>
+    <t>MetricModel_MetricEnum_PlayerLoad</t>
+  </si>
+  <si>
+    <t>プレーヤーロード</t>
+  </si>
+  <si>
+    <t>Player Load</t>
+  </si>
+  <si>
+    <t>MetricModel_MetricEnum_PlayerLoadPerMin</t>
+  </si>
+  <si>
+    <t>平均プレーヤーロード</t>
+  </si>
+  <si>
+    <t>Player Load Avg</t>
+  </si>
+  <si>
+    <t>MetricModel_MetricEnum_BaseBallScore1</t>
+  </si>
+  <si>
+    <t>MetricModel_MetricEnum_BaseBallScore2</t>
+  </si>
+  <si>
+    <t>MetricModel_MetricEnum_BaseBallScore3</t>
   </si>
   <si>
     <t>Message_Link_Copy_Success</t>
@@ -16055,7 +16082,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -16079,12 +16106,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="ＭＳ ゴシック"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -16115,7 +16136,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -16131,12 +16152,6 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -16458,20 +16473,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H1318"/>
+  <dimension ref="A1:H1323"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="49.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="49.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="45.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="49.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="49.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -16558,7 +16573,7 @@
       <c r="A6" s="1" t="s">
         <v>3194</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>326</v>
       </c>
       <c r="C6" s="1" t="s">
@@ -16574,7 +16589,7 @@
       <c r="A7" s="1" t="s">
         <v>3196</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>1706</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -17380,13 +17395,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="19.5">
       <c r="A59" s="1" t="s">
-        <v>713</v>
+        <v>3212</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>714</v>
+        <v>3213</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>715</v>
+        <v>3214</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
@@ -17396,13 +17411,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="19.5">
       <c r="A60" s="1" t="s">
-        <v>716</v>
+        <v>3215</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>717</v>
+        <v>3216</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>718</v>
+        <v>3217</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -17412,13 +17427,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="19.5">
       <c r="A61" s="1" t="s">
-        <v>719</v>
+        <v>3218</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>720</v>
+        <v>3203</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>721</v>
+        <v>3204</v>
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
@@ -17428,13 +17443,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="19.5">
       <c r="A62" s="1" t="s">
-        <v>722</v>
+        <v>3219</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>723</v>
+        <v>3207</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>724</v>
+        <v>3208</v>
       </c>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
@@ -17444,13 +17459,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="19.5">
       <c r="A63" s="1" t="s">
-        <v>725</v>
+        <v>3220</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>726</v>
+        <v>3210</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>727</v>
+        <v>3211</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
@@ -17460,13 +17475,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="19.5">
       <c r="A64" s="1" t="s">
-        <v>728</v>
+        <v>713</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>729</v>
+        <v>714</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>730</v>
+        <v>715</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
@@ -17476,13 +17491,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="19.5">
       <c r="A65" s="1" t="s">
-        <v>731</v>
+        <v>716</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>732</v>
+        <v>717</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>733</v>
+        <v>718</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
@@ -17492,13 +17507,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="19.5">
       <c r="A66" s="1" t="s">
-        <v>734</v>
+        <v>719</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>735</v>
+        <v>720</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>736</v>
+        <v>721</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
@@ -17508,13 +17523,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="19.5">
       <c r="A67" s="1" t="s">
-        <v>737</v>
+        <v>722</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>738</v>
+        <v>723</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>739</v>
+        <v>724</v>
       </c>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
@@ -17524,13 +17539,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="19.5">
       <c r="A68" s="1" t="s">
-        <v>740</v>
+        <v>725</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>741</v>
+        <v>726</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>742</v>
+        <v>727</v>
       </c>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
@@ -17540,13 +17555,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="19.5">
       <c r="A69" s="1" t="s">
-        <v>743</v>
+        <v>728</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>744</v>
+        <v>729</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>745</v>
+        <v>730</v>
       </c>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
@@ -17554,15 +17569,15 @@
       <c r="G69" s="3"/>
       <c r="H69" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="23.25">
       <c r="A70" s="1" t="s">
-        <v>746</v>
+        <v>731</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>747</v>
+        <v>732</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>748</v>
+        <v>733</v>
       </c>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
@@ -17570,15 +17585,15 @@
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="23.25">
       <c r="A71" s="1" t="s">
-        <v>749</v>
+        <v>734</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>750</v>
+        <v>735</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>751</v>
+        <v>736</v>
       </c>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
@@ -17586,15 +17601,15 @@
       <c r="G71" s="3"/>
       <c r="H71" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="23.25">
       <c r="A72" s="1" t="s">
-        <v>752</v>
+        <v>737</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>753</v>
+        <v>738</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>754</v>
+        <v>739</v>
       </c>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
@@ -17602,15 +17617,15 @@
       <c r="G72" s="3"/>
       <c r="H72" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="23.25">
       <c r="A73" s="1" t="s">
-        <v>755</v>
+        <v>740</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>756</v>
+        <v>741</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>757</v>
+        <v>742</v>
       </c>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
@@ -17618,15 +17633,15 @@
       <c r="G73" s="3"/>
       <c r="H73" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="23.25">
       <c r="A74" s="1" t="s">
-        <v>758</v>
+        <v>743</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>759</v>
+        <v>744</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>760</v>
+        <v>745</v>
       </c>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
@@ -17634,15 +17649,15 @@
       <c r="G74" s="3"/>
       <c r="H74" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="23.25">
       <c r="A75" s="1" t="s">
-        <v>761</v>
+        <v>746</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>762</v>
+        <v>747</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>763</v>
+        <v>748</v>
       </c>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
@@ -17650,15 +17665,15 @@
       <c r="G75" s="3"/>
       <c r="H75" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="23.25">
       <c r="A76" s="1" t="s">
-        <v>764</v>
+        <v>749</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>765</v>
+        <v>750</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>766</v>
+        <v>751</v>
       </c>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
@@ -17666,15 +17681,15 @@
       <c r="G76" s="3"/>
       <c r="H76" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="23.25">
       <c r="A77" s="1" t="s">
-        <v>767</v>
+        <v>752</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>768</v>
+        <v>753</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>769</v>
+        <v>754</v>
       </c>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
@@ -17682,15 +17697,15 @@
       <c r="G77" s="3"/>
       <c r="H77" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="23.25">
       <c r="A78" s="1" t="s">
-        <v>770</v>
+        <v>755</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>771</v>
+        <v>756</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>772</v>
+        <v>757</v>
       </c>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
@@ -17698,175 +17713,175 @@
       <c r="G78" s="3"/>
       <c r="H78" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="23.25">
       <c r="A79" s="1" t="s">
-        <v>773</v>
+        <v>758</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>774</v>
+        <v>759</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>444</v>
+        <v>760</v>
       </c>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
-      <c r="F79" s="1"/>
-      <c r="G79" s="1"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
       <c r="H79" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="23.25">
       <c r="A80" s="1" t="s">
-        <v>775</v>
+        <v>761</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>776</v>
+        <v>762</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>447</v>
+        <v>763</v>
       </c>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
-      <c r="F80" s="1"/>
-      <c r="G80" s="1"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
       <c r="H80" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="23.25">
       <c r="A81" s="1" t="s">
-        <v>777</v>
+        <v>764</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>778</v>
+        <v>765</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>450</v>
+        <v>766</v>
       </c>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="F81" s="1"/>
-      <c r="G81" s="1"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
       <c r="H81" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="23.25">
       <c r="A82" s="1" t="s">
-        <v>779</v>
+        <v>767</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>780</v>
+        <v>768</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>453</v>
+        <v>769</v>
       </c>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
-      <c r="F82" s="1"/>
-      <c r="G82" s="1"/>
+      <c r="F82" s="3"/>
+      <c r="G82" s="3"/>
       <c r="H82" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="23.25">
       <c r="A83" s="1" t="s">
-        <v>781</v>
+        <v>770</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>782</v>
+        <v>771</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>456</v>
+        <v>772</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
-      <c r="F83" s="1"/>
-      <c r="G83" s="1"/>
+      <c r="F83" s="3"/>
+      <c r="G83" s="3"/>
       <c r="H83" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="23.25">
       <c r="A84" s="1" t="s">
-        <v>783</v>
+        <v>773</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>784</v>
+        <v>774</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>459</v>
+        <v>444</v>
       </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
-      <c r="F84" s="3"/>
-      <c r="G84" s="3"/>
+      <c r="F84" s="1"/>
+      <c r="G84" s="1"/>
       <c r="H84" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="23.25">
       <c r="A85" s="1" t="s">
-        <v>785</v>
+        <v>775</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>786</v>
+        <v>776</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>787</v>
+        <v>447</v>
       </c>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
-      <c r="F85" s="3"/>
-      <c r="G85" s="3"/>
+      <c r="F85" s="1"/>
+      <c r="G85" s="1"/>
       <c r="H85" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="23.25">
       <c r="A86" s="1" t="s">
-        <v>788</v>
+        <v>777</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>789</v>
+        <v>778</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>790</v>
+        <v>450</v>
       </c>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
-      <c r="F86" s="3"/>
-      <c r="G86" s="3"/>
+      <c r="F86" s="1"/>
+      <c r="G86" s="1"/>
       <c r="H86" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="23.25">
       <c r="A87" s="1" t="s">
-        <v>791</v>
+        <v>779</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>792</v>
+        <v>780</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>793</v>
+        <v>453</v>
       </c>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
-      <c r="F87" s="3"/>
-      <c r="G87" s="3"/>
+      <c r="F87" s="1"/>
+      <c r="G87" s="1"/>
       <c r="H87" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="23.25">
       <c r="A88" s="1" t="s">
-        <v>794</v>
+        <v>781</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>795</v>
+        <v>782</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>796</v>
+        <v>456</v>
       </c>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="3"/>
-      <c r="G88" s="3"/>
+      <c r="F88" s="1"/>
+      <c r="G88" s="1"/>
       <c r="H88" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="23.25">
       <c r="A89" s="1" t="s">
-        <v>797</v>
+        <v>783</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>798</v>
+        <v>784</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>799</v>
+        <v>459</v>
       </c>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
@@ -17874,15 +17889,15 @@
       <c r="G89" s="3"/>
       <c r="H89" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="23.25">
       <c r="A90" s="1" t="s">
-        <v>800</v>
+        <v>785</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>801</v>
+        <v>786</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>802</v>
+        <v>787</v>
       </c>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
@@ -17890,15 +17905,15 @@
       <c r="G90" s="3"/>
       <c r="H90" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="23.25">
       <c r="A91" s="1" t="s">
-        <v>803</v>
+        <v>788</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>804</v>
+        <v>789</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>805</v>
+        <v>790</v>
       </c>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
@@ -17906,15 +17921,15 @@
       <c r="G91" s="3"/>
       <c r="H91" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="23.25">
       <c r="A92" s="1" t="s">
-        <v>806</v>
+        <v>791</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>807</v>
+        <v>792</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>808</v>
+        <v>793</v>
       </c>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
@@ -17922,15 +17937,15 @@
       <c r="G92" s="3"/>
       <c r="H92" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="23.25">
       <c r="A93" s="1" t="s">
-        <v>809</v>
+        <v>794</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>810</v>
+        <v>795</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>811</v>
+        <v>796</v>
       </c>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
@@ -17940,13 +17955,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="19.5">
       <c r="A94" s="1" t="s">
-        <v>812</v>
+        <v>797</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>813</v>
+        <v>798</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>814</v>
+        <v>799</v>
       </c>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
@@ -17956,13 +17971,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="19.5">
       <c r="A95" s="1" t="s">
-        <v>815</v>
+        <v>800</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>816</v>
+        <v>801</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>817</v>
+        <v>802</v>
       </c>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
@@ -17972,13 +17987,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="19.5">
       <c r="A96" s="1" t="s">
-        <v>818</v>
+        <v>803</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>819</v>
+        <v>804</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>820</v>
+        <v>805</v>
       </c>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
@@ -17988,13 +18003,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="19.5">
       <c r="A97" s="1" t="s">
-        <v>821</v>
+        <v>806</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>822</v>
+        <v>807</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>823</v>
+        <v>808</v>
       </c>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
@@ -18004,13 +18019,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="19.5">
       <c r="A98" s="1" t="s">
-        <v>824</v>
+        <v>809</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>825</v>
+        <v>810</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>826</v>
+        <v>811</v>
       </c>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
@@ -18020,13 +18035,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="19.5">
       <c r="A99" s="1" t="s">
-        <v>827</v>
+        <v>812</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>828</v>
+        <v>813</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>829</v>
+        <v>814</v>
       </c>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
@@ -18036,13 +18051,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="19.5">
       <c r="A100" s="1" t="s">
-        <v>830</v>
+        <v>815</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>831</v>
+        <v>816</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>832</v>
+        <v>817</v>
       </c>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
@@ -18052,13 +18067,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="19.5">
       <c r="A101" s="1" t="s">
-        <v>833</v>
+        <v>818</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>834</v>
+        <v>819</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>835</v>
+        <v>820</v>
       </c>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
@@ -18068,13 +18083,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="19.5">
       <c r="A102" s="1" t="s">
-        <v>836</v>
+        <v>821</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>837</v>
+        <v>822</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>838</v>
+        <v>823</v>
       </c>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
@@ -18084,13 +18099,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="19.5">
       <c r="A103" s="1" t="s">
-        <v>839</v>
+        <v>824</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>840</v>
+        <v>825</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>841</v>
+        <v>826</v>
       </c>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
@@ -18100,13 +18115,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="19.5">
       <c r="A104" s="1" t="s">
-        <v>842</v>
+        <v>827</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>843</v>
+        <v>828</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>844</v>
+        <v>829</v>
       </c>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
@@ -18116,13 +18131,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="19.5">
       <c r="A105" s="1" t="s">
-        <v>845</v>
+        <v>830</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>846</v>
+        <v>831</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>847</v>
+        <v>832</v>
       </c>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
@@ -18132,13 +18147,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="19.5">
       <c r="A106" s="1" t="s">
-        <v>848</v>
+        <v>833</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>849</v>
+        <v>834</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>850</v>
+        <v>835</v>
       </c>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
@@ -18148,13 +18163,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="19.5">
       <c r="A107" s="1" t="s">
-        <v>851</v>
+        <v>836</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>852</v>
+        <v>837</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>853</v>
+        <v>838</v>
       </c>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
@@ -18164,13 +18179,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="19.5">
       <c r="A108" s="1" t="s">
-        <v>854</v>
+        <v>839</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>855</v>
+        <v>840</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>856</v>
+        <v>841</v>
       </c>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
@@ -18179,9 +18194,15 @@
       <c r="H108" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="109" customHeight="1" ht="19.5">
-      <c r="A109" s="1"/>
-      <c r="B109" s="1"/>
-      <c r="C109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>844</v>
+      </c>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
       <c r="F109" s="3"/>
@@ -18190,13 +18211,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="110" customHeight="1" ht="19.5">
       <c r="A110" s="1" t="s">
-        <v>3212</v>
-      </c>
-      <c r="B110" s="4" t="s">
-        <v>3213</v>
+        <v>845</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>846</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>3214</v>
+        <v>847</v>
       </c>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
@@ -18206,13 +18227,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="111" customHeight="1" ht="19.5">
       <c r="A111" s="1" t="s">
-        <v>108</v>
+        <v>848</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>109</v>
+        <v>849</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>110</v>
+        <v>850</v>
       </c>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
@@ -18222,13 +18243,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="112" customHeight="1" ht="19.5">
       <c r="A112" s="1" t="s">
-        <v>111</v>
+        <v>851</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>112</v>
+        <v>852</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>113</v>
+        <v>853</v>
       </c>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
@@ -18238,13 +18259,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="113" customHeight="1" ht="19.5">
       <c r="A113" s="1" t="s">
-        <v>114</v>
+        <v>854</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>115</v>
+        <v>855</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>116</v>
+        <v>856</v>
       </c>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
@@ -18253,15 +18274,9 @@
       <c r="H113" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="114" customHeight="1" ht="19.5">
-      <c r="A114" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="B114" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="C114" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="1"/>
+      <c r="C114" s="1"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
       <c r="F114" s="3"/>
@@ -18270,13 +18285,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="115" customHeight="1" ht="19.5">
       <c r="A115" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="B115" s="1" t="s">
-        <v>121</v>
+        <v>3221</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>3222</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>122</v>
+        <v>3223</v>
       </c>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
@@ -18286,13 +18301,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="116" customHeight="1" ht="19.5">
       <c r="A116" s="1" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
@@ -18302,13 +18317,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="117" customHeight="1" ht="19.5">
       <c r="A117" s="1" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
@@ -18318,13 +18333,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="118" customHeight="1" ht="19.5">
       <c r="A118" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
@@ -18334,13 +18349,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="119" customHeight="1" ht="19.5">
       <c r="A119" s="1" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>134</v>
+        <v>119</v>
       </c>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
@@ -18350,13 +18365,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="120" customHeight="1" ht="19.5">
       <c r="A120" s="1" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
@@ -18366,13 +18381,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="121" customHeight="1" ht="19.5">
       <c r="A121" s="1" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
@@ -18382,13 +18397,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="122" customHeight="1" ht="19.5">
       <c r="A122" s="1" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
@@ -18398,13 +18413,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="123" customHeight="1" ht="19.5">
       <c r="A123" s="1" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
@@ -18414,13 +18429,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="124" customHeight="1" ht="19.5">
       <c r="A124" s="1" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
@@ -18430,13 +18445,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="125" customHeight="1" ht="19.5">
       <c r="A125" s="1" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
@@ -18446,13 +18461,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="126" customHeight="1" ht="19.5">
       <c r="A126" s="1" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
@@ -18462,13 +18477,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="127" customHeight="1" ht="19.5">
       <c r="A127" s="1" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
@@ -18478,13 +18493,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="128" customHeight="1" ht="19.5">
       <c r="A128" s="1" t="s">
-        <v>159</v>
+        <v>144</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>160</v>
+        <v>145</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>104</v>
+        <v>146</v>
       </c>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
@@ -18494,13 +18509,13 @@
     </row>
     <row x14ac:dyDescent="0.25" r="129" customHeight="1" ht="19.5">
       <c r="A129" s="1" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
@@ -18509,9 +18524,15 @@
       <c r="H129" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="130" customHeight="1" ht="19.5">
-      <c r="A130" s="1"/>
-      <c r="B130" s="1"/>
-      <c r="C130" s="1"/>
+      <c r="A130" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="B130" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>152</v>
+      </c>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
       <c r="F130" s="3"/>
@@ -18519,9 +18540,15 @@
       <c r="H130" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
-      <c r="A131" s="1"/>
-      <c r="B131" s="1"/>
-      <c r="C131" s="1"/>
+      <c r="A131" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C131" s="1" t="s">
+        <v>155</v>
+      </c>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
       <c r="F131" s="3"/>
@@ -18529,9 +18556,15 @@
       <c r="H131" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="132" customHeight="1" ht="19.5">
-      <c r="A132" s="1"/>
-      <c r="B132" s="1"/>
-      <c r="C132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B132" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
       <c r="F132" s="3"/>
@@ -18539,9 +18572,15 @@
       <c r="H132" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="133" customHeight="1" ht="19.5">
-      <c r="A133" s="1"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="1"/>
+      <c r="A133" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
       <c r="F133" s="3"/>
@@ -18549,9 +18588,15 @@
       <c r="H133" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="134" customHeight="1" ht="19.5">
-      <c r="A134" s="1"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="1"/>
+      <c r="A134" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C134" s="1" t="s">
+        <v>163</v>
+      </c>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
       <c r="F134" s="3"/>
@@ -18600,7 +18645,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="139" customHeight="1" ht="19.5">
       <c r="A139" s="1"/>
-      <c r="B139" s="1"/>
+      <c r="B139" s="2"/>
       <c r="C139" s="1"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
@@ -18620,7 +18665,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="141" customHeight="1" ht="19.5">
       <c r="A141" s="1"/>
-      <c r="B141" s="2"/>
+      <c r="B141" s="1"/>
       <c r="C141" s="1"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
@@ -18630,7 +18675,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="142" customHeight="1" ht="19.5">
       <c r="A142" s="1"/>
-      <c r="B142" s="2"/>
+      <c r="B142" s="1"/>
       <c r="C142" s="1"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
@@ -18640,7 +18685,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="143" customHeight="1" ht="19.5">
       <c r="A143" s="1"/>
-      <c r="B143" s="1"/>
+      <c r="B143" s="2"/>
       <c r="C143" s="1"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
@@ -18670,7 +18715,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="146" customHeight="1" ht="19.5">
       <c r="A146" s="1"/>
-      <c r="B146" s="1"/>
+      <c r="B146" s="2"/>
       <c r="C146" s="1"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
@@ -18680,7 +18725,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="147" customHeight="1" ht="19.5">
       <c r="A147" s="1"/>
-      <c r="B147" s="1"/>
+      <c r="B147" s="2"/>
       <c r="C147" s="1"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
@@ -18690,7 +18735,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="148" customHeight="1" ht="19.5">
       <c r="A148" s="1"/>
-      <c r="B148" s="2"/>
+      <c r="B148" s="1"/>
       <c r="C148" s="1"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
@@ -18700,8 +18745,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="149" customHeight="1" ht="19.5">
       <c r="A149" s="1"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
+      <c r="B149" s="1"/>
+      <c r="C149" s="1"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
       <c r="F149" s="3"/>
@@ -18740,7 +18785,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="153" customHeight="1" ht="19.5">
       <c r="A153" s="1"/>
-      <c r="B153" s="1"/>
+      <c r="B153" s="2"/>
       <c r="C153" s="1"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
@@ -18750,8 +18795,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="154" customHeight="1" ht="19.5">
       <c r="A154" s="1"/>
-      <c r="B154" s="1"/>
-      <c r="C154" s="1"/>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
       <c r="F154" s="3"/>
@@ -18780,8 +18825,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="157" customHeight="1" ht="19.5">
       <c r="A157" s="1"/>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
+      <c r="B157" s="1"/>
+      <c r="C157" s="1"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
       <c r="F157" s="3"/>
@@ -18790,8 +18835,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="158" customHeight="1" ht="19.5">
       <c r="A158" s="1"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
+      <c r="B158" s="1"/>
+      <c r="C158" s="1"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
       <c r="F158" s="3"/>
@@ -18800,8 +18845,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="159" customHeight="1" ht="19.5">
       <c r="A159" s="1"/>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
+      <c r="B159" s="1"/>
+      <c r="C159" s="1"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
       <c r="F159" s="3"/>
@@ -18810,8 +18855,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="160" customHeight="1" ht="19.5">
       <c r="A160" s="1"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
+      <c r="B160" s="1"/>
+      <c r="C160" s="1"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
       <c r="F160" s="3"/>
@@ -18820,8 +18865,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="161" customHeight="1" ht="19.5">
       <c r="A161" s="1"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
       <c r="F161" s="3"/>
@@ -18881,7 +18926,7 @@
     <row x14ac:dyDescent="0.25" r="167" customHeight="1" ht="19.5">
       <c r="A167" s="1"/>
       <c r="B167" s="2"/>
-      <c r="C167" s="1"/>
+      <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
       <c r="F167" s="3"/>
@@ -18891,7 +18936,7 @@
     <row x14ac:dyDescent="0.25" r="168" customHeight="1" ht="19.5">
       <c r="A168" s="1"/>
       <c r="B168" s="2"/>
-      <c r="C168" s="1"/>
+      <c r="C168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
       <c r="F168" s="3"/>
@@ -18901,7 +18946,7 @@
     <row x14ac:dyDescent="0.25" r="169" customHeight="1" ht="19.5">
       <c r="A169" s="1"/>
       <c r="B169" s="2"/>
-      <c r="C169" s="1"/>
+      <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
       <c r="F169" s="3"/>
@@ -18911,7 +18956,7 @@
     <row x14ac:dyDescent="0.25" r="170" customHeight="1" ht="19.5">
       <c r="A170" s="1"/>
       <c r="B170" s="2"/>
-      <c r="C170" s="1"/>
+      <c r="C170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
       <c r="F170" s="3"/>
@@ -18921,7 +18966,7 @@
     <row x14ac:dyDescent="0.25" r="171" customHeight="1" ht="19.5">
       <c r="A171" s="1"/>
       <c r="B171" s="2"/>
-      <c r="C171" s="1"/>
+      <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
       <c r="F171" s="3"/>
@@ -18931,7 +18976,7 @@
     <row x14ac:dyDescent="0.25" r="172" customHeight="1" ht="19.5">
       <c r="A172" s="1"/>
       <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
+      <c r="C172" s="1"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
       <c r="F172" s="3"/>
@@ -18941,7 +18986,7 @@
     <row x14ac:dyDescent="0.25" r="173" customHeight="1" ht="19.5">
       <c r="A173" s="1"/>
       <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
+      <c r="C173" s="1"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
       <c r="F173" s="3"/>
@@ -18951,7 +18996,7 @@
     <row x14ac:dyDescent="0.25" r="174" customHeight="1" ht="19.5">
       <c r="A174" s="1"/>
       <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
+      <c r="C174" s="1"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
       <c r="F174" s="3"/>
@@ -18961,7 +19006,7 @@
     <row x14ac:dyDescent="0.25" r="175" customHeight="1" ht="19.5">
       <c r="A175" s="1"/>
       <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
+      <c r="C175" s="1"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
       <c r="F175" s="3"/>
@@ -18970,7 +19015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="176" customHeight="1" ht="19.5">
       <c r="A176" s="1"/>
-      <c r="B176" s="1"/>
+      <c r="B176" s="2"/>
       <c r="C176" s="1"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
@@ -18980,18 +19025,18 @@
     </row>
     <row x14ac:dyDescent="0.25" r="177" customHeight="1" ht="19.5">
       <c r="A177" s="1"/>
-      <c r="B177" s="1"/>
-      <c r="C177" s="1"/>
+      <c r="B177" s="2"/>
+      <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
       <c r="F177" s="3"/>
       <c r="G177" s="3"/>
       <c r="H177" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="178" customHeight="1" ht="19.5">
       <c r="A178" s="1"/>
-      <c r="B178" s="1"/>
-      <c r="C178" s="1"/>
+      <c r="B178" s="2"/>
+      <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
       <c r="F178" s="3"/>
@@ -19000,25 +19045,25 @@
     </row>
     <row x14ac:dyDescent="0.25" r="179" customHeight="1" ht="19.5">
       <c r="A179" s="1"/>
-      <c r="B179" s="1"/>
-      <c r="C179" s="1"/>
+      <c r="B179" s="2"/>
+      <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
       <c r="F179" s="3"/>
       <c r="G179" s="3"/>
       <c r="H179" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="180" customHeight="1" ht="19.5">
       <c r="A180" s="1"/>
-      <c r="B180" s="1"/>
-      <c r="C180" s="1"/>
+      <c r="B180" s="2"/>
+      <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
       <c r="F180" s="3"/>
       <c r="G180" s="3"/>
       <c r="H180" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="181" customHeight="1" ht="19.5">
       <c r="A181" s="1"/>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -19028,7 +19073,7 @@
       <c r="G181" s="3"/>
       <c r="H181" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="182" customHeight="1" ht="19.5">
       <c r="A182" s="1"/>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -19048,7 +19093,7 @@
       <c r="G183" s="3"/>
       <c r="H183" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="184" customHeight="1" ht="19.5">
       <c r="A184" s="1"/>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -19128,50 +19173,50 @@
       <c r="G191" s="3"/>
       <c r="H191" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="192" customHeight="1" ht="21.75">
       <c r="A192" s="1"/>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
+      <c r="B192" s="1"/>
+      <c r="C192" s="1"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
       <c r="F192" s="3"/>
       <c r="G192" s="3"/>
       <c r="H192" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="193" customHeight="1" ht="21.75">
       <c r="A193" s="1"/>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
+      <c r="B193" s="1"/>
+      <c r="C193" s="1"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
       <c r="F193" s="3"/>
       <c r="G193" s="3"/>
       <c r="H193" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="194" customHeight="1" ht="21.75">
       <c r="A194" s="1"/>
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
+      <c r="B194" s="1"/>
+      <c r="C194" s="1"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
       <c r="F194" s="3"/>
       <c r="G194" s="3"/>
       <c r="H194" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="195" customHeight="1" ht="21.75">
       <c r="A195" s="1"/>
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
+      <c r="B195" s="1"/>
+      <c r="C195" s="1"/>
       <c r="D195" s="2"/>
       <c r="E195" s="2"/>
       <c r="F195" s="3"/>
       <c r="G195" s="3"/>
       <c r="H195" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="196" customHeight="1" ht="21.75">
       <c r="A196" s="1"/>
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
+      <c r="B196" s="1"/>
+      <c r="C196" s="1"/>
       <c r="D196" s="2"/>
       <c r="E196" s="2"/>
       <c r="F196" s="3"/>
@@ -19278,20 +19323,20 @@
       <c r="G206" s="3"/>
       <c r="H206" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="207" customHeight="1" ht="19.5">
       <c r="A207" s="1"/>
-      <c r="B207" s="1"/>
-      <c r="C207" s="1"/>
+      <c r="B207" s="2"/>
+      <c r="C207" s="2"/>
       <c r="D207" s="2"/>
       <c r="E207" s="2"/>
       <c r="F207" s="3"/>
       <c r="G207" s="3"/>
       <c r="H207" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="19.5">
       <c r="A208" s="1"/>
-      <c r="B208" s="1"/>
-      <c r="C208" s="1"/>
+      <c r="B208" s="2"/>
+      <c r="C208" s="2"/>
       <c r="D208" s="2"/>
       <c r="E208" s="2"/>
       <c r="F208" s="3"/>
@@ -19310,8 +19355,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="19.5">
       <c r="A210" s="1"/>
-      <c r="B210" s="1"/>
-      <c r="C210" s="1"/>
+      <c r="B210" s="2"/>
+      <c r="C210" s="2"/>
       <c r="D210" s="2"/>
       <c r="E210" s="2"/>
       <c r="F210" s="3"/>
@@ -19320,15 +19365,15 @@
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="19.5">
       <c r="A211" s="1"/>
-      <c r="B211" s="1"/>
-      <c r="C211" s="1"/>
+      <c r="B211" s="2"/>
+      <c r="C211" s="2"/>
       <c r="D211" s="2"/>
       <c r="E211" s="2"/>
       <c r="F211" s="3"/>
       <c r="G211" s="3"/>
       <c r="H211" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="21.75">
       <c r="A212" s="1"/>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -19338,7 +19383,7 @@
       <c r="G212" s="3"/>
       <c r="H212" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="21.75">
       <c r="A213" s="1"/>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -19360,8 +19405,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="215" customHeight="1" ht="19.5">
       <c r="A215" s="1"/>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
+      <c r="B215" s="1"/>
+      <c r="C215" s="1"/>
       <c r="D215" s="2"/>
       <c r="E215" s="2"/>
       <c r="F215" s="3"/>
@@ -19400,8 +19445,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="219" customHeight="1" ht="19.5">
       <c r="A219" s="1"/>
-      <c r="B219" s="1"/>
-      <c r="C219" s="1"/>
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
       <c r="D219" s="2"/>
       <c r="E219" s="2"/>
       <c r="F219" s="3"/>
@@ -19420,7 +19465,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="221" customHeight="1" ht="19.5">
       <c r="A221" s="1"/>
-      <c r="B221" s="2"/>
+      <c r="B221" s="1"/>
       <c r="C221" s="1"/>
       <c r="D221" s="2"/>
       <c r="E221" s="2"/>
@@ -19430,7 +19475,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="222" customHeight="1" ht="19.5">
       <c r="A222" s="1"/>
-      <c r="B222" s="2"/>
+      <c r="B222" s="1"/>
       <c r="C222" s="1"/>
       <c r="D222" s="2"/>
       <c r="E222" s="2"/>
@@ -19440,7 +19485,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="223" customHeight="1" ht="19.5">
       <c r="A223" s="1"/>
-      <c r="B223" s="2"/>
+      <c r="B223" s="1"/>
       <c r="C223" s="1"/>
       <c r="D223" s="2"/>
       <c r="E223" s="2"/>
@@ -19450,7 +19495,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="224" customHeight="1" ht="19.5">
       <c r="A224" s="1"/>
-      <c r="B224" s="2"/>
+      <c r="B224" s="1"/>
       <c r="C224" s="1"/>
       <c r="D224" s="2"/>
       <c r="E224" s="2"/>
@@ -19461,7 +19506,7 @@
     <row x14ac:dyDescent="0.25" r="225" customHeight="1" ht="19.5">
       <c r="A225" s="1"/>
       <c r="B225" s="2"/>
-      <c r="C225" s="1"/>
+      <c r="C225" s="2"/>
       <c r="D225" s="2"/>
       <c r="E225" s="2"/>
       <c r="F225" s="3"/>
@@ -19471,7 +19516,7 @@
     <row x14ac:dyDescent="0.25" r="226" customHeight="1" ht="19.5">
       <c r="A226" s="1"/>
       <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
+      <c r="C226" s="1"/>
       <c r="D226" s="2"/>
       <c r="E226" s="2"/>
       <c r="F226" s="3"/>
@@ -19481,7 +19526,7 @@
     <row x14ac:dyDescent="0.25" r="227" customHeight="1" ht="19.5">
       <c r="A227" s="1"/>
       <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
+      <c r="C227" s="1"/>
       <c r="D227" s="2"/>
       <c r="E227" s="2"/>
       <c r="F227" s="3"/>
@@ -19491,7 +19536,7 @@
     <row x14ac:dyDescent="0.25" r="228" customHeight="1" ht="19.5">
       <c r="A228" s="1"/>
       <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
+      <c r="C228" s="1"/>
       <c r="D228" s="2"/>
       <c r="E228" s="2"/>
       <c r="F228" s="3"/>
@@ -19501,7 +19546,7 @@
     <row x14ac:dyDescent="0.25" r="229" customHeight="1" ht="19.5">
       <c r="A229" s="1"/>
       <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
+      <c r="C229" s="1"/>
       <c r="D229" s="2"/>
       <c r="E229" s="2"/>
       <c r="F229" s="3"/>
@@ -19511,7 +19556,7 @@
     <row x14ac:dyDescent="0.25" r="230" customHeight="1" ht="19.5">
       <c r="A230" s="1"/>
       <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
+      <c r="C230" s="1"/>
       <c r="D230" s="2"/>
       <c r="E230" s="2"/>
       <c r="F230" s="3"/>
@@ -19520,8 +19565,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="231" customHeight="1" ht="19.5">
       <c r="A231" s="1"/>
-      <c r="B231" s="1"/>
-      <c r="C231" s="1"/>
+      <c r="B231" s="2"/>
+      <c r="C231" s="2"/>
       <c r="D231" s="2"/>
       <c r="E231" s="2"/>
       <c r="F231" s="3"/>
@@ -19530,8 +19575,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="232" customHeight="1" ht="19.5">
       <c r="A232" s="1"/>
-      <c r="B232" s="1"/>
-      <c r="C232" s="1"/>
+      <c r="B232" s="2"/>
+      <c r="C232" s="2"/>
       <c r="D232" s="2"/>
       <c r="E232" s="2"/>
       <c r="F232" s="3"/>
@@ -19540,8 +19585,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="233" customHeight="1" ht="19.5">
       <c r="A233" s="1"/>
-      <c r="B233" s="1"/>
-      <c r="C233" s="1"/>
+      <c r="B233" s="2"/>
+      <c r="C233" s="2"/>
       <c r="D233" s="2"/>
       <c r="E233" s="2"/>
       <c r="F233" s="3"/>
@@ -19550,8 +19595,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="234" customHeight="1" ht="19.5">
       <c r="A234" s="1"/>
-      <c r="B234" s="1"/>
-      <c r="C234" s="1"/>
+      <c r="B234" s="2"/>
+      <c r="C234" s="2"/>
       <c r="D234" s="2"/>
       <c r="E234" s="2"/>
       <c r="F234" s="3"/>
@@ -19560,8 +19605,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="235" customHeight="1" ht="19.5">
       <c r="A235" s="1"/>
-      <c r="B235" s="1"/>
-      <c r="C235" s="1"/>
+      <c r="B235" s="2"/>
+      <c r="C235" s="2"/>
       <c r="D235" s="2"/>
       <c r="E235" s="2"/>
       <c r="F235" s="3"/>
@@ -19650,8 +19695,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="244" customHeight="1" ht="19.5">
       <c r="A244" s="1"/>
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
+      <c r="B244" s="1"/>
+      <c r="C244" s="1"/>
       <c r="D244" s="2"/>
       <c r="E244" s="2"/>
       <c r="F244" s="3"/>
@@ -19660,8 +19705,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="245" customHeight="1" ht="19.5">
       <c r="A245" s="1"/>
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
+      <c r="B245" s="1"/>
+      <c r="C245" s="1"/>
       <c r="D245" s="2"/>
       <c r="E245" s="2"/>
       <c r="F245" s="3"/>
@@ -19670,8 +19715,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="246" customHeight="1" ht="19.5">
       <c r="A246" s="1"/>
-      <c r="B246" s="2"/>
-      <c r="C246" s="2"/>
+      <c r="B246" s="1"/>
+      <c r="C246" s="1"/>
       <c r="D246" s="2"/>
       <c r="E246" s="2"/>
       <c r="F246" s="3"/>
@@ -19680,8 +19725,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="247" customHeight="1" ht="19.5">
       <c r="A247" s="1"/>
-      <c r="B247" s="2"/>
-      <c r="C247" s="2"/>
+      <c r="B247" s="1"/>
+      <c r="C247" s="1"/>
       <c r="D247" s="2"/>
       <c r="E247" s="2"/>
       <c r="F247" s="3"/>
@@ -19690,8 +19735,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="248" customHeight="1" ht="19.5">
       <c r="A248" s="1"/>
-      <c r="B248" s="2"/>
-      <c r="C248" s="2"/>
+      <c r="B248" s="1"/>
+      <c r="C248" s="1"/>
       <c r="D248" s="2"/>
       <c r="E248" s="2"/>
       <c r="F248" s="3"/>
@@ -19800,8 +19845,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="259" customHeight="1" ht="19.5">
       <c r="A259" s="1"/>
-      <c r="B259" s="1"/>
-      <c r="C259" s="1"/>
+      <c r="B259" s="2"/>
+      <c r="C259" s="2"/>
       <c r="D259" s="2"/>
       <c r="E259" s="2"/>
       <c r="F259" s="3"/>
@@ -19810,8 +19855,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="260" customHeight="1" ht="19.5">
       <c r="A260" s="1"/>
-      <c r="B260" s="1"/>
-      <c r="C260" s="1"/>
+      <c r="B260" s="2"/>
+      <c r="C260" s="2"/>
       <c r="D260" s="2"/>
       <c r="E260" s="2"/>
       <c r="F260" s="3"/>
@@ -19820,7 +19865,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="261" customHeight="1" ht="19.5">
       <c r="A261" s="1"/>
-      <c r="B261" s="1"/>
+      <c r="B261" s="2"/>
       <c r="C261" s="2"/>
       <c r="D261" s="2"/>
       <c r="E261" s="2"/>
@@ -19830,7 +19875,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="262" customHeight="1" ht="19.5">
       <c r="A262" s="1"/>
-      <c r="B262" s="1"/>
+      <c r="B262" s="2"/>
       <c r="C262" s="2"/>
       <c r="D262" s="2"/>
       <c r="E262" s="2"/>
@@ -19840,8 +19885,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="263" customHeight="1" ht="19.5">
       <c r="A263" s="1"/>
-      <c r="B263" s="1"/>
-      <c r="C263" s="1"/>
+      <c r="B263" s="2"/>
+      <c r="C263" s="2"/>
       <c r="D263" s="2"/>
       <c r="E263" s="2"/>
       <c r="F263" s="3"/>
@@ -19871,7 +19916,7 @@
     <row x14ac:dyDescent="0.25" r="266" customHeight="1" ht="19.5">
       <c r="A266" s="1"/>
       <c r="B266" s="1"/>
-      <c r="C266" s="1"/>
+      <c r="C266" s="2"/>
       <c r="D266" s="2"/>
       <c r="E266" s="2"/>
       <c r="F266" s="3"/>
@@ -19881,7 +19926,7 @@
     <row x14ac:dyDescent="0.25" r="267" customHeight="1" ht="19.5">
       <c r="A267" s="1"/>
       <c r="B267" s="1"/>
-      <c r="C267" s="1"/>
+      <c r="C267" s="2"/>
       <c r="D267" s="2"/>
       <c r="E267" s="2"/>
       <c r="F267" s="3"/>
@@ -20030,7 +20075,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="282" customHeight="1" ht="19.5">
       <c r="A282" s="1"/>
-      <c r="B282" s="2"/>
+      <c r="B282" s="1"/>
       <c r="C282" s="1"/>
       <c r="D282" s="2"/>
       <c r="E282" s="2"/>
@@ -20080,7 +20125,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="287" customHeight="1" ht="19.5">
       <c r="A287" s="1"/>
-      <c r="B287" s="1"/>
+      <c r="B287" s="2"/>
       <c r="C287" s="1"/>
       <c r="D287" s="2"/>
       <c r="E287" s="2"/>
@@ -20850,8 +20895,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="364" customHeight="1" ht="19.5">
       <c r="A364" s="1"/>
-      <c r="B364" s="2"/>
-      <c r="C364" s="2"/>
+      <c r="B364" s="1"/>
+      <c r="C364" s="1"/>
       <c r="D364" s="2"/>
       <c r="E364" s="2"/>
       <c r="F364" s="3"/>
@@ -20860,8 +20905,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="365" customHeight="1" ht="19.5">
       <c r="A365" s="1"/>
-      <c r="B365" s="2"/>
-      <c r="C365" s="2"/>
+      <c r="B365" s="1"/>
+      <c r="C365" s="1"/>
       <c r="D365" s="2"/>
       <c r="E365" s="2"/>
       <c r="F365" s="3"/>
@@ -20870,8 +20915,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="366" customHeight="1" ht="19.5">
       <c r="A366" s="1"/>
-      <c r="B366" s="2"/>
-      <c r="C366" s="2"/>
+      <c r="B366" s="1"/>
+      <c r="C366" s="1"/>
       <c r="D366" s="2"/>
       <c r="E366" s="2"/>
       <c r="F366" s="3"/>
@@ -20880,8 +20925,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="367" customHeight="1" ht="19.5">
       <c r="A367" s="1"/>
-      <c r="B367" s="2"/>
-      <c r="C367" s="2"/>
+      <c r="B367" s="1"/>
+      <c r="C367" s="1"/>
       <c r="D367" s="2"/>
       <c r="E367" s="2"/>
       <c r="F367" s="3"/>
@@ -20890,8 +20935,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="368" customHeight="1" ht="19.5">
       <c r="A368" s="1"/>
-      <c r="B368" s="2"/>
-      <c r="C368" s="2"/>
+      <c r="B368" s="1"/>
+      <c r="C368" s="1"/>
       <c r="D368" s="2"/>
       <c r="E368" s="2"/>
       <c r="F368" s="3"/>
@@ -21619,19 +21664,19 @@
       <c r="H440" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="19.5">
-      <c r="A441" s="6"/>
-      <c r="B441" s="6"/>
-      <c r="C441" s="6"/>
-      <c r="D441" s="7"/>
-      <c r="E441" s="7"/>
+      <c r="A441" s="1"/>
+      <c r="B441" s="2"/>
+      <c r="C441" s="2"/>
+      <c r="D441" s="2"/>
+      <c r="E441" s="2"/>
       <c r="F441" s="3"/>
       <c r="G441" s="3"/>
       <c r="H441" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="442" customHeight="1" ht="19.5">
       <c r="A442" s="1"/>
-      <c r="B442" s="1"/>
-      <c r="C442" s="1"/>
+      <c r="B442" s="2"/>
+      <c r="C442" s="2"/>
       <c r="D442" s="2"/>
       <c r="E442" s="2"/>
       <c r="F442" s="3"/>
@@ -21688,20 +21733,20 @@
       <c r="G447" s="3"/>
       <c r="H447" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="448" customHeight="1" ht="19.5" customFormat="1" s="8">
-      <c r="A448" s="2"/>
+    <row x14ac:dyDescent="0.25" r="448" customHeight="1" ht="19.5">
+      <c r="A448" s="1"/>
       <c r="B448" s="2"/>
       <c r="C448" s="2"/>
       <c r="D448" s="2"/>
       <c r="E448" s="2"/>
-      <c r="F448" s="2"/>
-      <c r="G448" s="2"/>
-      <c r="H448" s="2"/>
+      <c r="F448" s="3"/>
+      <c r="G448" s="3"/>
+      <c r="H448" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="449" customHeight="1" ht="19.5">
       <c r="A449" s="1"/>
-      <c r="B449" s="1"/>
-      <c r="C449" s="1"/>
+      <c r="B449" s="2"/>
+      <c r="C449" s="2"/>
       <c r="D449" s="2"/>
       <c r="E449" s="2"/>
       <c r="F449" s="3"/>
@@ -21710,8 +21755,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="450" customHeight="1" ht="19.5">
       <c r="A450" s="1"/>
-      <c r="B450" s="1"/>
-      <c r="C450" s="1"/>
+      <c r="B450" s="2"/>
+      <c r="C450" s="2"/>
       <c r="D450" s="2"/>
       <c r="E450" s="2"/>
       <c r="F450" s="3"/>
@@ -21730,7 +21775,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="452" customHeight="1" ht="19.5">
       <c r="A452" s="1"/>
-      <c r="B452" s="4"/>
+      <c r="B452" s="1"/>
       <c r="C452" s="1"/>
       <c r="D452" s="2"/>
       <c r="E452" s="2"/>
@@ -21738,19 +21783,19 @@
       <c r="G452" s="3"/>
       <c r="H452" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="19.5">
-      <c r="A453" s="1"/>
-      <c r="B453" s="4"/>
-      <c r="C453" s="1"/>
+    <row x14ac:dyDescent="0.25" r="453" customHeight="1" ht="19.5" customFormat="1" s="6">
+      <c r="A453" s="2"/>
+      <c r="B453" s="2"/>
+      <c r="C453" s="2"/>
       <c r="D453" s="2"/>
       <c r="E453" s="2"/>
-      <c r="F453" s="3"/>
-      <c r="G453" s="3"/>
-      <c r="H453" s="3"/>
+      <c r="F453" s="2"/>
+      <c r="G453" s="2"/>
+      <c r="H453" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="454" customHeight="1" ht="19.5">
       <c r="A454" s="1"/>
-      <c r="B454" s="4"/>
+      <c r="B454" s="1"/>
       <c r="C454" s="1"/>
       <c r="D454" s="2"/>
       <c r="E454" s="2"/>
@@ -21760,7 +21805,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="455" customHeight="1" ht="19.5">
       <c r="A455" s="1"/>
-      <c r="B455" s="4"/>
+      <c r="B455" s="1"/>
       <c r="C455" s="1"/>
       <c r="D455" s="2"/>
       <c r="E455" s="2"/>
@@ -21780,7 +21825,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="457" customHeight="1" ht="19.5">
       <c r="A457" s="1"/>
-      <c r="B457" s="1"/>
+      <c r="B457" s="4"/>
       <c r="C457" s="1"/>
       <c r="D457" s="2"/>
       <c r="E457" s="2"/>
@@ -21790,7 +21835,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="458" customHeight="1" ht="19.5">
       <c r="A458" s="1"/>
-      <c r="B458" s="1"/>
+      <c r="B458" s="4"/>
       <c r="C458" s="1"/>
       <c r="D458" s="2"/>
       <c r="E458" s="2"/>
@@ -21800,7 +21845,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="459" customHeight="1" ht="19.5">
       <c r="A459" s="1"/>
-      <c r="B459" s="1"/>
+      <c r="B459" s="4"/>
       <c r="C459" s="1"/>
       <c r="D459" s="2"/>
       <c r="E459" s="2"/>
@@ -21810,7 +21855,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="460" customHeight="1" ht="19.5">
       <c r="A460" s="1"/>
-      <c r="B460" s="1"/>
+      <c r="B460" s="4"/>
       <c r="C460" s="1"/>
       <c r="D460" s="2"/>
       <c r="E460" s="2"/>
@@ -21940,7 +21985,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="473" customHeight="1" ht="19.5">
       <c r="A473" s="1"/>
-      <c r="B473" s="2"/>
+      <c r="B473" s="1"/>
       <c r="C473" s="1"/>
       <c r="D473" s="2"/>
       <c r="E473" s="2"/>
@@ -21950,7 +21995,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="474" customHeight="1" ht="19.5">
       <c r="A474" s="1"/>
-      <c r="B474" s="2"/>
+      <c r="B474" s="1"/>
       <c r="C474" s="1"/>
       <c r="D474" s="2"/>
       <c r="E474" s="2"/>
@@ -21960,7 +22005,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="475" customHeight="1" ht="19.5">
       <c r="A475" s="1"/>
-      <c r="B475" s="2"/>
+      <c r="B475" s="1"/>
       <c r="C475" s="1"/>
       <c r="D475" s="2"/>
       <c r="E475" s="2"/>
@@ -21970,7 +22015,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="476" customHeight="1" ht="19.5">
       <c r="A476" s="1"/>
-      <c r="B476" s="2"/>
+      <c r="B476" s="1"/>
       <c r="C476" s="1"/>
       <c r="D476" s="2"/>
       <c r="E476" s="2"/>
@@ -21980,8 +22025,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="477" customHeight="1" ht="19.5">
       <c r="A477" s="1"/>
-      <c r="B477" s="2"/>
-      <c r="C477" s="2"/>
+      <c r="B477" s="1"/>
+      <c r="C477" s="1"/>
       <c r="D477" s="2"/>
       <c r="E477" s="2"/>
       <c r="F477" s="3"/>
@@ -21991,7 +22036,7 @@
     <row x14ac:dyDescent="0.25" r="478" customHeight="1" ht="19.5">
       <c r="A478" s="1"/>
       <c r="B478" s="2"/>
-      <c r="C478" s="2"/>
+      <c r="C478" s="1"/>
       <c r="D478" s="2"/>
       <c r="E478" s="2"/>
       <c r="F478" s="3"/>
@@ -22001,7 +22046,7 @@
     <row x14ac:dyDescent="0.25" r="479" customHeight="1" ht="19.5">
       <c r="A479" s="1"/>
       <c r="B479" s="2"/>
-      <c r="C479" s="2"/>
+      <c r="C479" s="1"/>
       <c r="D479" s="2"/>
       <c r="E479" s="2"/>
       <c r="F479" s="3"/>
@@ -22010,7 +22055,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="480" customHeight="1" ht="19.5">
       <c r="A480" s="1"/>
-      <c r="B480" s="9"/>
+      <c r="B480" s="2"/>
       <c r="C480" s="1"/>
       <c r="D480" s="2"/>
       <c r="E480" s="2"/>
@@ -22020,7 +22065,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="481" customHeight="1" ht="19.5">
       <c r="A481" s="1"/>
-      <c r="B481" s="9"/>
+      <c r="B481" s="2"/>
       <c r="C481" s="1"/>
       <c r="D481" s="2"/>
       <c r="E481" s="2"/>
@@ -22030,8 +22075,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="482" customHeight="1" ht="19.5">
       <c r="A482" s="1"/>
-      <c r="B482" s="1"/>
-      <c r="C482" s="1"/>
+      <c r="B482" s="2"/>
+      <c r="C482" s="2"/>
       <c r="D482" s="2"/>
       <c r="E482" s="2"/>
       <c r="F482" s="3"/>
@@ -22040,8 +22085,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="483" customHeight="1" ht="19.5">
       <c r="A483" s="1"/>
-      <c r="B483" s="1"/>
-      <c r="C483" s="1"/>
+      <c r="B483" s="2"/>
+      <c r="C483" s="2"/>
       <c r="D483" s="2"/>
       <c r="E483" s="2"/>
       <c r="F483" s="3"/>
@@ -22050,8 +22095,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="484" customHeight="1" ht="19.5">
       <c r="A484" s="1"/>
-      <c r="B484" s="9"/>
-      <c r="C484" s="1"/>
+      <c r="B484" s="2"/>
+      <c r="C484" s="2"/>
       <c r="D484" s="2"/>
       <c r="E484" s="2"/>
       <c r="F484" s="3"/>
@@ -22060,7 +22105,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="485" customHeight="1" ht="19.5">
       <c r="A485" s="1"/>
-      <c r="B485" s="2"/>
+      <c r="B485" s="7"/>
       <c r="C485" s="1"/>
       <c r="D485" s="2"/>
       <c r="E485" s="2"/>
@@ -22070,7 +22115,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="486" customHeight="1" ht="19.5">
       <c r="A486" s="1"/>
-      <c r="B486" s="9"/>
+      <c r="B486" s="7"/>
       <c r="C486" s="1"/>
       <c r="D486" s="2"/>
       <c r="E486" s="2"/>
@@ -22100,7 +22145,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="489" customHeight="1" ht="19.5">
       <c r="A489" s="1"/>
-      <c r="B489" s="1"/>
+      <c r="B489" s="7"/>
       <c r="C489" s="1"/>
       <c r="D489" s="2"/>
       <c r="E489" s="2"/>
@@ -22110,7 +22155,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="490" customHeight="1" ht="19.5">
       <c r="A490" s="1"/>
-      <c r="B490" s="1"/>
+      <c r="B490" s="2"/>
       <c r="C490" s="1"/>
       <c r="D490" s="2"/>
       <c r="E490" s="2"/>
@@ -22120,7 +22165,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="491" customHeight="1" ht="19.5">
       <c r="A491" s="1"/>
-      <c r="B491" s="1"/>
+      <c r="B491" s="7"/>
       <c r="C491" s="1"/>
       <c r="D491" s="2"/>
       <c r="E491" s="2"/>
@@ -22130,7 +22175,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="492" customHeight="1" ht="19.5">
       <c r="A492" s="1"/>
-      <c r="B492" s="2"/>
+      <c r="B492" s="1"/>
       <c r="C492" s="1"/>
       <c r="D492" s="2"/>
       <c r="E492" s="2"/>
@@ -22140,7 +22185,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="493" customHeight="1" ht="19.5">
       <c r="A493" s="1"/>
-      <c r="B493" s="2"/>
+      <c r="B493" s="1"/>
       <c r="C493" s="1"/>
       <c r="D493" s="2"/>
       <c r="E493" s="2"/>
@@ -22150,7 +22195,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="494" customHeight="1" ht="19.5">
       <c r="A494" s="1"/>
-      <c r="B494" s="2"/>
+      <c r="B494" s="1"/>
       <c r="C494" s="1"/>
       <c r="D494" s="2"/>
       <c r="E494" s="2"/>
@@ -22160,7 +22205,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="495" customHeight="1" ht="19.5">
       <c r="A495" s="1"/>
-      <c r="B495" s="2"/>
+      <c r="B495" s="1"/>
       <c r="C495" s="1"/>
       <c r="D495" s="2"/>
       <c r="E495" s="2"/>
@@ -22170,7 +22215,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="496" customHeight="1" ht="19.5">
       <c r="A496" s="1"/>
-      <c r="B496" s="2"/>
+      <c r="B496" s="1"/>
       <c r="C496" s="1"/>
       <c r="D496" s="2"/>
       <c r="E496" s="2"/>
@@ -22210,7 +22255,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="500" customHeight="1" ht="19.5">
       <c r="A500" s="1"/>
-      <c r="B500" s="1"/>
+      <c r="B500" s="2"/>
       <c r="C500" s="1"/>
       <c r="D500" s="2"/>
       <c r="E500" s="2"/>
@@ -22258,12 +22303,12 @@
       <c r="G504" s="3"/>
       <c r="H504" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="505" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="505" customHeight="1" ht="19.5">
       <c r="A505" s="1"/>
-      <c r="B505" s="6"/>
-      <c r="C505" s="6"/>
-      <c r="D505" s="7"/>
-      <c r="E505" s="7"/>
+      <c r="B505" s="1"/>
+      <c r="C505" s="1"/>
+      <c r="D505" s="2"/>
+      <c r="E505" s="2"/>
       <c r="F505" s="3"/>
       <c r="G505" s="3"/>
       <c r="H505" s="3"/>
@@ -22308,9 +22353,9 @@
       <c r="G509" s="3"/>
       <c r="H509" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="510" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="510" customHeight="1" ht="18.75">
       <c r="A510" s="1"/>
-      <c r="B510" s="2"/>
+      <c r="B510" s="1"/>
       <c r="C510" s="1"/>
       <c r="D510" s="2"/>
       <c r="E510" s="2"/>
@@ -22320,7 +22365,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="511" customHeight="1" ht="19.5">
       <c r="A511" s="1"/>
-      <c r="B511" s="1"/>
+      <c r="B511" s="2"/>
       <c r="C511" s="1"/>
       <c r="D511" s="2"/>
       <c r="E511" s="2"/>
@@ -22330,41 +22375,41 @@
     </row>
     <row x14ac:dyDescent="0.25" r="512" customHeight="1" ht="19.5">
       <c r="A512" s="1"/>
-      <c r="B512" s="1"/>
+      <c r="B512" s="2"/>
       <c r="C512" s="1"/>
       <c r="D512" s="2"/>
       <c r="E512" s="2"/>
-      <c r="F512" s="1"/>
+      <c r="F512" s="3"/>
       <c r="G512" s="3"/>
       <c r="H512" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="513" customHeight="1" ht="19.5">
       <c r="A513" s="1"/>
-      <c r="B513" s="1"/>
+      <c r="B513" s="2"/>
       <c r="C513" s="1"/>
       <c r="D513" s="2"/>
       <c r="E513" s="2"/>
-      <c r="F513" s="1"/>
+      <c r="F513" s="3"/>
       <c r="G513" s="3"/>
       <c r="H513" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="514" customHeight="1" ht="19.5">
       <c r="A514" s="1"/>
-      <c r="B514" s="1"/>
+      <c r="B514" s="2"/>
       <c r="C514" s="1"/>
       <c r="D514" s="2"/>
       <c r="E514" s="2"/>
-      <c r="F514" s="1"/>
+      <c r="F514" s="3"/>
       <c r="G514" s="3"/>
       <c r="H514" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="515" customHeight="1" ht="19.5">
       <c r="A515" s="1"/>
-      <c r="B515" s="1"/>
+      <c r="B515" s="2"/>
       <c r="C515" s="1"/>
       <c r="D515" s="2"/>
       <c r="E515" s="2"/>
-      <c r="F515" s="1"/>
+      <c r="F515" s="3"/>
       <c r="G515" s="3"/>
       <c r="H515" s="3"/>
     </row>
@@ -22374,7 +22419,7 @@
       <c r="C516" s="1"/>
       <c r="D516" s="2"/>
       <c r="E516" s="2"/>
-      <c r="F516" s="1"/>
+      <c r="F516" s="3"/>
       <c r="G516" s="3"/>
       <c r="H516" s="3"/>
     </row>
@@ -22384,9 +22429,7 @@
       <c r="C517" s="1"/>
       <c r="D517" s="2"/>
       <c r="E517" s="2"/>
-      <c r="F517" s="1" t="s">
-        <v>1278</v>
-      </c>
+      <c r="F517" s="1"/>
       <c r="G517" s="3"/>
       <c r="H517" s="3"/>
     </row>
@@ -22436,7 +22479,9 @@
       <c r="C522" s="1"/>
       <c r="D522" s="2"/>
       <c r="E522" s="2"/>
-      <c r="F522" s="1"/>
+      <c r="F522" s="1" t="s">
+        <v>1278</v>
+      </c>
       <c r="G522" s="3"/>
       <c r="H522" s="3"/>
     </row>
@@ -22472,7 +22517,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="526" customHeight="1" ht="19.5">
       <c r="A526" s="1"/>
-      <c r="B526" s="2"/>
+      <c r="B526" s="1"/>
       <c r="C526" s="1"/>
       <c r="D526" s="2"/>
       <c r="E526" s="2"/>
@@ -22482,7 +22527,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="527" customHeight="1" ht="19.5">
       <c r="A527" s="1"/>
-      <c r="B527" s="2"/>
+      <c r="B527" s="1"/>
       <c r="C527" s="1"/>
       <c r="D527" s="2"/>
       <c r="E527" s="2"/>
@@ -22492,7 +22537,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="528" customHeight="1" ht="19.5">
       <c r="A528" s="1"/>
-      <c r="B528" s="2"/>
+      <c r="B528" s="1"/>
       <c r="C528" s="1"/>
       <c r="D528" s="2"/>
       <c r="E528" s="2"/>
@@ -22502,7 +22547,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="529" customHeight="1" ht="19.5">
       <c r="A529" s="1"/>
-      <c r="B529" s="2"/>
+      <c r="B529" s="1"/>
       <c r="C529" s="1"/>
       <c r="D529" s="2"/>
       <c r="E529" s="2"/>
@@ -22516,17 +22561,17 @@
       <c r="C530" s="1"/>
       <c r="D530" s="2"/>
       <c r="E530" s="2"/>
-      <c r="F530" s="3"/>
+      <c r="F530" s="1"/>
       <c r="G530" s="3"/>
       <c r="H530" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="531" customHeight="1" ht="19.5">
       <c r="A531" s="1"/>
-      <c r="B531" s="1"/>
+      <c r="B531" s="2"/>
       <c r="C531" s="1"/>
       <c r="D531" s="2"/>
       <c r="E531" s="2"/>
-      <c r="F531" s="3"/>
+      <c r="F531" s="1"/>
       <c r="G531" s="3"/>
       <c r="H531" s="3"/>
     </row>
@@ -22536,7 +22581,7 @@
       <c r="C532" s="1"/>
       <c r="D532" s="2"/>
       <c r="E532" s="2"/>
-      <c r="F532" s="3"/>
+      <c r="F532" s="1"/>
       <c r="G532" s="3"/>
       <c r="H532" s="3"/>
     </row>
@@ -22546,7 +22591,7 @@
       <c r="C533" s="1"/>
       <c r="D533" s="2"/>
       <c r="E533" s="2"/>
-      <c r="F533" s="3"/>
+      <c r="F533" s="1"/>
       <c r="G533" s="3"/>
       <c r="H533" s="3"/>
     </row>
@@ -22556,13 +22601,13 @@
       <c r="C534" s="1"/>
       <c r="D534" s="2"/>
       <c r="E534" s="2"/>
-      <c r="F534" s="3"/>
+      <c r="F534" s="1"/>
       <c r="G534" s="3"/>
       <c r="H534" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="535" customHeight="1" ht="19.5">
       <c r="A535" s="1"/>
-      <c r="B535" s="2"/>
+      <c r="B535" s="1"/>
       <c r="C535" s="1"/>
       <c r="D535" s="2"/>
       <c r="E535" s="2"/>
@@ -22572,7 +22617,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="536" customHeight="1" ht="19.5">
       <c r="A536" s="1"/>
-      <c r="B536" s="2"/>
+      <c r="B536" s="1"/>
       <c r="C536" s="1"/>
       <c r="D536" s="2"/>
       <c r="E536" s="2"/>
@@ -22592,7 +22637,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="538" customHeight="1" ht="19.5">
       <c r="A538" s="1"/>
-      <c r="B538" s="1"/>
+      <c r="B538" s="2"/>
       <c r="C538" s="1"/>
       <c r="D538" s="2"/>
       <c r="E538" s="2"/>
@@ -22602,7 +22647,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="539" customHeight="1" ht="19.5">
       <c r="A539" s="1"/>
-      <c r="B539" s="1"/>
+      <c r="B539" s="2"/>
       <c r="C539" s="1"/>
       <c r="D539" s="2"/>
       <c r="E539" s="2"/>
@@ -22612,7 +22657,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="540" customHeight="1" ht="19.5">
       <c r="A540" s="1"/>
-      <c r="B540" s="1"/>
+      <c r="B540" s="2"/>
       <c r="C540" s="1"/>
       <c r="D540" s="2"/>
       <c r="E540" s="2"/>
@@ -22622,7 +22667,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="541" customHeight="1" ht="19.5">
       <c r="A541" s="1"/>
-      <c r="B541" s="1"/>
+      <c r="B541" s="2"/>
       <c r="C541" s="1"/>
       <c r="D541" s="2"/>
       <c r="E541" s="2"/>
@@ -22632,7 +22677,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="542" customHeight="1" ht="19.5">
       <c r="A542" s="1"/>
-      <c r="B542" s="1"/>
+      <c r="B542" s="2"/>
       <c r="C542" s="1"/>
       <c r="D542" s="2"/>
       <c r="E542" s="2"/>
@@ -22692,37 +22737,37 @@
     </row>
     <row x14ac:dyDescent="0.25" r="548" customHeight="1" ht="19.5">
       <c r="A548" s="1"/>
-      <c r="B548" s="2"/>
-      <c r="C548" s="2"/>
+      <c r="B548" s="1"/>
+      <c r="C548" s="1"/>
       <c r="D548" s="2"/>
       <c r="E548" s="2"/>
       <c r="F548" s="3"/>
       <c r="G548" s="3"/>
       <c r="H548" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="549" customHeight="1" ht="37.5">
+    <row x14ac:dyDescent="0.25" r="549" customHeight="1" ht="19.5">
       <c r="A549" s="1"/>
-      <c r="B549" s="2"/>
-      <c r="C549" s="2"/>
+      <c r="B549" s="1"/>
+      <c r="C549" s="1"/>
       <c r="D549" s="2"/>
       <c r="E549" s="2"/>
       <c r="F549" s="3"/>
       <c r="G549" s="3"/>
       <c r="H549" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="550" customHeight="1" ht="37.5">
+    <row x14ac:dyDescent="0.25" r="550" customHeight="1" ht="19.5">
       <c r="A550" s="1"/>
-      <c r="B550" s="2"/>
-      <c r="C550" s="2"/>
+      <c r="B550" s="1"/>
+      <c r="C550" s="1"/>
       <c r="D550" s="2"/>
       <c r="E550" s="2"/>
-      <c r="F550" s="2"/>
-      <c r="G550" s="2"/>
-      <c r="H550" s="2"/>
+      <c r="F550" s="3"/>
+      <c r="G550" s="3"/>
+      <c r="H550" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="551" customHeight="1" ht="19.5">
       <c r="A551" s="1"/>
-      <c r="B551" s="2"/>
+      <c r="B551" s="1"/>
       <c r="C551" s="1"/>
       <c r="D551" s="2"/>
       <c r="E551" s="2"/>
@@ -22732,7 +22777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="552" customHeight="1" ht="19.5">
       <c r="A552" s="1"/>
-      <c r="B552" s="9"/>
+      <c r="B552" s="1"/>
       <c r="C552" s="1"/>
       <c r="D552" s="2"/>
       <c r="E552" s="2"/>
@@ -22742,7 +22787,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="553" customHeight="1" ht="19.5">
       <c r="A553" s="1"/>
-      <c r="B553" s="9"/>
+      <c r="B553" s="2"/>
       <c r="C553" s="2"/>
       <c r="D553" s="2"/>
       <c r="E553" s="2"/>
@@ -22750,53 +22795,53 @@
       <c r="G553" s="3"/>
       <c r="H553" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="554" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="554" customHeight="1" ht="37.5">
       <c r="A554" s="1"/>
       <c r="B554" s="2"/>
-      <c r="C554" s="1"/>
+      <c r="C554" s="2"/>
       <c r="D554" s="2"/>
       <c r="E554" s="2"/>
       <c r="F554" s="3"/>
       <c r="G554" s="3"/>
       <c r="H554" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="555" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="555" customHeight="1" ht="37.5">
       <c r="A555" s="1"/>
       <c r="B555" s="2"/>
       <c r="C555" s="2"/>
       <c r="D555" s="2"/>
       <c r="E555" s="2"/>
-      <c r="F555" s="3"/>
-      <c r="G555" s="3"/>
-      <c r="H555" s="3"/>
+      <c r="F555" s="2"/>
+      <c r="G555" s="2"/>
+      <c r="H555" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="556" customHeight="1" ht="19.5">
       <c r="A556" s="1"/>
       <c r="B556" s="2"/>
-      <c r="C556" s="2"/>
+      <c r="C556" s="1"/>
       <c r="D556" s="2"/>
       <c r="E556" s="2"/>
       <c r="F556" s="3"/>
       <c r="G556" s="3"/>
       <c r="H556" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="557" customHeight="1" ht="37.5" customFormat="1" s="8">
-      <c r="A557" s="2"/>
-      <c r="B557" s="2"/>
-      <c r="C557" s="2"/>
+    <row x14ac:dyDescent="0.25" r="557" customHeight="1" ht="19.5">
+      <c r="A557" s="1"/>
+      <c r="B557" s="7"/>
+      <c r="C557" s="1"/>
       <c r="D557" s="2"/>
       <c r="E557" s="2"/>
-      <c r="F557" s="2"/>
-      <c r="G557" s="2"/>
-      <c r="H557" s="2"/>
+      <c r="F557" s="3"/>
+      <c r="G557" s="3"/>
+      <c r="H557" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="558" customHeight="1" ht="19.5">
       <c r="A558" s="1"/>
-      <c r="B558" s="2"/>
-      <c r="C558" s="1"/>
+      <c r="B558" s="7"/>
+      <c r="C558" s="2"/>
       <c r="D558" s="2"/>
       <c r="E558" s="2"/>
-      <c r="F558" s="1"/>
+      <c r="F558" s="3"/>
       <c r="G558" s="3"/>
       <c r="H558" s="3"/>
     </row>
@@ -22806,73 +22851,73 @@
       <c r="C559" s="1"/>
       <c r="D559" s="2"/>
       <c r="E559" s="2"/>
-      <c r="F559" s="1"/>
+      <c r="F559" s="3"/>
       <c r="G559" s="3"/>
       <c r="H559" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="560" customHeight="1" ht="19.5">
       <c r="A560" s="1"/>
       <c r="B560" s="2"/>
-      <c r="C560" s="1"/>
+      <c r="C560" s="2"/>
       <c r="D560" s="2"/>
       <c r="E560" s="2"/>
-      <c r="F560" s="1"/>
+      <c r="F560" s="3"/>
       <c r="G560" s="3"/>
       <c r="H560" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="561" customHeight="1" ht="19.5">
       <c r="A561" s="1"/>
-      <c r="B561" s="1"/>
-      <c r="C561" s="1"/>
+      <c r="B561" s="2"/>
+      <c r="C561" s="2"/>
       <c r="D561" s="2"/>
       <c r="E561" s="2"/>
       <c r="F561" s="3"/>
       <c r="G561" s="3"/>
       <c r="H561" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="562" customHeight="1" ht="39.75">
-      <c r="A562" s="1"/>
+    <row x14ac:dyDescent="0.25" r="562" customHeight="1" ht="37.5" customFormat="1" s="6">
+      <c r="A562" s="2"/>
       <c r="B562" s="2"/>
-      <c r="C562" s="1"/>
+      <c r="C562" s="2"/>
       <c r="D562" s="2"/>
       <c r="E562" s="2"/>
-      <c r="F562" s="3"/>
-      <c r="G562" s="3"/>
-      <c r="H562" s="3"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="563" customHeight="1" ht="39.75">
+      <c r="F562" s="2"/>
+      <c r="G562" s="2"/>
+      <c r="H562" s="2"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="563" customHeight="1" ht="19.5">
       <c r="A563" s="1"/>
       <c r="B563" s="2"/>
       <c r="C563" s="1"/>
       <c r="D563" s="2"/>
       <c r="E563" s="2"/>
-      <c r="F563" s="3"/>
+      <c r="F563" s="1"/>
       <c r="G563" s="3"/>
       <c r="H563" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="564" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="564" customHeight="1" ht="19.5">
       <c r="A564" s="1"/>
-      <c r="B564" s="10"/>
+      <c r="B564" s="2"/>
       <c r="C564" s="1"/>
       <c r="D564" s="2"/>
       <c r="E564" s="2"/>
-      <c r="F564" s="3"/>
+      <c r="F564" s="1"/>
       <c r="G564" s="3"/>
       <c r="H564" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="565" customHeight="1" ht="39.75">
+    <row x14ac:dyDescent="0.25" r="565" customHeight="1" ht="19.5">
       <c r="A565" s="1"/>
-      <c r="B565" s="10"/>
+      <c r="B565" s="2"/>
       <c r="C565" s="1"/>
       <c r="D565" s="2"/>
       <c r="E565" s="2"/>
-      <c r="F565" s="3"/>
+      <c r="F565" s="1"/>
       <c r="G565" s="3"/>
       <c r="H565" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="566" customHeight="1" ht="19.5">
       <c r="A566" s="1"/>
-      <c r="B566" s="5"/>
+      <c r="B566" s="1"/>
       <c r="C566" s="1"/>
       <c r="D566" s="2"/>
       <c r="E566" s="2"/>
@@ -22880,9 +22925,9 @@
       <c r="G566" s="3"/>
       <c r="H566" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="567" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="567" customHeight="1" ht="39.75">
       <c r="A567" s="1"/>
-      <c r="B567" s="5"/>
+      <c r="B567" s="2"/>
       <c r="C567" s="1"/>
       <c r="D567" s="2"/>
       <c r="E567" s="2"/>
@@ -22890,7 +22935,7 @@
       <c r="G567" s="3"/>
       <c r="H567" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="568" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="568" customHeight="1" ht="39.75">
       <c r="A568" s="1"/>
       <c r="B568" s="2"/>
       <c r="C568" s="1"/>
@@ -22900,9 +22945,9 @@
       <c r="G568" s="3"/>
       <c r="H568" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="569" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="569" customHeight="1" ht="39.75">
       <c r="A569" s="1"/>
-      <c r="B569" s="2"/>
+      <c r="B569" s="8"/>
       <c r="C569" s="1"/>
       <c r="D569" s="2"/>
       <c r="E569" s="2"/>
@@ -22910,9 +22955,9 @@
       <c r="G569" s="3"/>
       <c r="H569" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="570" customHeight="1" ht="19.5">
+    <row x14ac:dyDescent="0.25" r="570" customHeight="1" ht="39.75">
       <c r="A570" s="1"/>
-      <c r="B570" s="2"/>
+      <c r="B570" s="8"/>
       <c r="C570" s="1"/>
       <c r="D570" s="2"/>
       <c r="E570" s="2"/>
@@ -22922,7 +22967,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="571" customHeight="1" ht="19.5">
       <c r="A571" s="1"/>
-      <c r="B571" s="2"/>
+      <c r="B571" s="5"/>
       <c r="C571" s="1"/>
       <c r="D571" s="2"/>
       <c r="E571" s="2"/>
@@ -22932,7 +22977,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="572" customHeight="1" ht="19.5">
       <c r="A572" s="1"/>
-      <c r="B572" s="2"/>
+      <c r="B572" s="5"/>
       <c r="C572" s="1"/>
       <c r="D572" s="2"/>
       <c r="E572" s="2"/>
@@ -23082,7 +23127,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="587" customHeight="1" ht="19.5">
       <c r="A587" s="1"/>
-      <c r="B587" s="1"/>
+      <c r="B587" s="2"/>
       <c r="C587" s="1"/>
       <c r="D587" s="2"/>
       <c r="E587" s="2"/>
@@ -23092,7 +23137,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="588" customHeight="1" ht="19.5">
       <c r="A588" s="1"/>
-      <c r="B588" s="1"/>
+      <c r="B588" s="2"/>
       <c r="C588" s="1"/>
       <c r="D588" s="2"/>
       <c r="E588" s="2"/>
@@ -23102,7 +23147,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="589" customHeight="1" ht="19.5">
       <c r="A589" s="1"/>
-      <c r="B589" s="1"/>
+      <c r="B589" s="2"/>
       <c r="C589" s="1"/>
       <c r="D589" s="2"/>
       <c r="E589" s="2"/>
@@ -23112,7 +23157,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="590" customHeight="1" ht="19.5">
       <c r="A590" s="1"/>
-      <c r="B590" s="1"/>
+      <c r="B590" s="2"/>
       <c r="C590" s="1"/>
       <c r="D590" s="2"/>
       <c r="E590" s="2"/>
@@ -23122,7 +23167,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="591" customHeight="1" ht="19.5">
       <c r="A591" s="1"/>
-      <c r="B591" s="1"/>
+      <c r="B591" s="2"/>
       <c r="C591" s="1"/>
       <c r="D591" s="2"/>
       <c r="E591" s="2"/>
@@ -23772,8 +23817,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="656" customHeight="1" ht="19.5">
       <c r="A656" s="1"/>
-      <c r="B656" s="2"/>
-      <c r="C656" s="2"/>
+      <c r="B656" s="1"/>
+      <c r="C656" s="1"/>
       <c r="D656" s="2"/>
       <c r="E656" s="2"/>
       <c r="F656" s="3"/>
@@ -23782,8 +23827,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="657" customHeight="1" ht="19.5">
       <c r="A657" s="1"/>
-      <c r="B657" s="2"/>
-      <c r="C657" s="2"/>
+      <c r="B657" s="1"/>
+      <c r="C657" s="1"/>
       <c r="D657" s="2"/>
       <c r="E657" s="2"/>
       <c r="F657" s="3"/>
@@ -23812,8 +23857,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="660" customHeight="1" ht="19.5">
       <c r="A660" s="1"/>
-      <c r="B660" s="2"/>
-      <c r="C660" s="2"/>
+      <c r="B660" s="1"/>
+      <c r="C660" s="1"/>
       <c r="D660" s="2"/>
       <c r="E660" s="2"/>
       <c r="F660" s="3"/>
@@ -23822,8 +23867,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="661" customHeight="1" ht="19.5">
       <c r="A661" s="1"/>
-      <c r="B661" s="1"/>
-      <c r="C661" s="1"/>
+      <c r="B661" s="2"/>
+      <c r="C661" s="2"/>
       <c r="D661" s="2"/>
       <c r="E661" s="2"/>
       <c r="F661" s="3"/>
@@ -23832,8 +23877,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="662" customHeight="1" ht="19.5">
       <c r="A662" s="1"/>
-      <c r="B662" s="1"/>
-      <c r="C662" s="1"/>
+      <c r="B662" s="2"/>
+      <c r="C662" s="2"/>
       <c r="D662" s="2"/>
       <c r="E662" s="2"/>
       <c r="F662" s="3"/>
@@ -23862,8 +23907,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="665" customHeight="1" ht="19.5">
       <c r="A665" s="1"/>
-      <c r="B665" s="1"/>
-      <c r="C665" s="1"/>
+      <c r="B665" s="2"/>
+      <c r="C665" s="2"/>
       <c r="D665" s="2"/>
       <c r="E665" s="2"/>
       <c r="F665" s="3"/>
@@ -24041,11 +24086,11 @@
       <c r="H682" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="683" customHeight="1" ht="19.5">
-      <c r="A683" s="6"/>
-      <c r="B683" s="6"/>
-      <c r="C683" s="6"/>
-      <c r="D683" s="7"/>
-      <c r="E683" s="7"/>
+      <c r="A683" s="1"/>
+      <c r="B683" s="1"/>
+      <c r="C683" s="1"/>
+      <c r="D683" s="2"/>
+      <c r="E683" s="2"/>
       <c r="F683" s="3"/>
       <c r="G683" s="3"/>
       <c r="H683" s="3"/>
@@ -24412,8 +24457,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="720" customHeight="1" ht="19.5">
       <c r="A720" s="1"/>
-      <c r="B720" s="2"/>
-      <c r="C720" s="2"/>
+      <c r="B720" s="1"/>
+      <c r="C720" s="1"/>
       <c r="D720" s="2"/>
       <c r="E720" s="2"/>
       <c r="F720" s="3"/>
@@ -24462,8 +24507,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="725" customHeight="1" ht="19.5">
       <c r="A725" s="1"/>
-      <c r="B725" s="1"/>
-      <c r="C725" s="1"/>
+      <c r="B725" s="2"/>
+      <c r="C725" s="2"/>
       <c r="D725" s="2"/>
       <c r="E725" s="2"/>
       <c r="F725" s="3"/>
@@ -25427,8 +25472,8 @@
       <c r="D821" s="2"/>
       <c r="E821" s="2"/>
       <c r="F821" s="3"/>
-      <c r="G821" s="1"/>
-      <c r="H821" s="1"/>
+      <c r="G821" s="3"/>
+      <c r="H821" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="822" customHeight="1" ht="19.5">
       <c r="A822" s="1"/>
@@ -25437,8 +25482,8 @@
       <c r="D822" s="2"/>
       <c r="E822" s="2"/>
       <c r="F822" s="3"/>
-      <c r="G822" s="1"/>
-      <c r="H822" s="1"/>
+      <c r="G822" s="3"/>
+      <c r="H822" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="823" customHeight="1" ht="19.5">
       <c r="A823" s="1"/>
@@ -25447,8 +25492,8 @@
       <c r="D823" s="2"/>
       <c r="E823" s="2"/>
       <c r="F823" s="3"/>
-      <c r="G823" s="1"/>
-      <c r="H823" s="1"/>
+      <c r="G823" s="3"/>
+      <c r="H823" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="824" customHeight="1" ht="19.5">
       <c r="A824" s="1"/>
@@ -25457,8 +25502,8 @@
       <c r="D824" s="2"/>
       <c r="E824" s="2"/>
       <c r="F824" s="3"/>
-      <c r="G824" s="1"/>
-      <c r="H824" s="1"/>
+      <c r="G824" s="3"/>
+      <c r="H824" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="825" customHeight="1" ht="19.5">
       <c r="A825" s="1"/>
@@ -25477,8 +25522,8 @@
       <c r="D826" s="2"/>
       <c r="E826" s="2"/>
       <c r="F826" s="3"/>
-      <c r="G826" s="3"/>
-      <c r="H826" s="3"/>
+      <c r="G826" s="1"/>
+      <c r="H826" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="827" customHeight="1" ht="19.5">
       <c r="A827" s="1"/>
@@ -25517,8 +25562,8 @@
       <c r="D830" s="2"/>
       <c r="E830" s="2"/>
       <c r="F830" s="3"/>
-      <c r="G830" s="1"/>
-      <c r="H830" s="1"/>
+      <c r="G830" s="3"/>
+      <c r="H830" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="831" customHeight="1" ht="19.5">
       <c r="A831" s="1"/>
@@ -25537,8 +25582,8 @@
       <c r="D832" s="2"/>
       <c r="E832" s="2"/>
       <c r="F832" s="3"/>
-      <c r="G832" s="3"/>
-      <c r="H832" s="3"/>
+      <c r="G832" s="1"/>
+      <c r="H832" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="833" customHeight="1" ht="19.5">
       <c r="A833" s="1"/>
@@ -25547,8 +25592,8 @@
       <c r="D833" s="2"/>
       <c r="E833" s="2"/>
       <c r="F833" s="3"/>
-      <c r="G833" s="3"/>
-      <c r="H833" s="3"/>
+      <c r="G833" s="1"/>
+      <c r="H833" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="834" customHeight="1" ht="19.5">
       <c r="A834" s="1"/>
@@ -25557,8 +25602,8 @@
       <c r="D834" s="2"/>
       <c r="E834" s="2"/>
       <c r="F834" s="3"/>
-      <c r="G834" s="3"/>
-      <c r="H834" s="3"/>
+      <c r="G834" s="1"/>
+      <c r="H834" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="835" customHeight="1" ht="19.5">
       <c r="A835" s="1"/>
@@ -25567,8 +25612,8 @@
       <c r="D835" s="2"/>
       <c r="E835" s="2"/>
       <c r="F835" s="3"/>
-      <c r="G835" s="3"/>
-      <c r="H835" s="3"/>
+      <c r="G835" s="1"/>
+      <c r="H835" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="836" customHeight="1" ht="19.5">
       <c r="A836" s="1"/>
@@ -26302,8 +26347,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="909" customHeight="1" ht="19.5">
       <c r="A909" s="1"/>
-      <c r="B909" s="2"/>
-      <c r="C909" s="2"/>
+      <c r="B909" s="1"/>
+      <c r="C909" s="1"/>
       <c r="D909" s="2"/>
       <c r="E909" s="2"/>
       <c r="F909" s="3"/>
@@ -26352,8 +26397,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="914" customHeight="1" ht="19.5">
       <c r="A914" s="1"/>
-      <c r="B914" s="1"/>
-      <c r="C914" s="1"/>
+      <c r="B914" s="2"/>
+      <c r="C914" s="2"/>
       <c r="D914" s="2"/>
       <c r="E914" s="2"/>
       <c r="F914" s="3"/>
@@ -27491,51 +27536,51 @@
       <c r="H1027" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1028" customHeight="1" ht="19.5">
-      <c r="A1028" s="6"/>
-      <c r="B1028" s="6"/>
-      <c r="C1028" s="6"/>
-      <c r="D1028" s="7"/>
-      <c r="E1028" s="7"/>
+      <c r="A1028" s="1"/>
+      <c r="B1028" s="1"/>
+      <c r="C1028" s="1"/>
+      <c r="D1028" s="2"/>
+      <c r="E1028" s="2"/>
       <c r="F1028" s="3"/>
       <c r="G1028" s="3"/>
       <c r="H1028" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1029" customHeight="1" ht="19.5">
-      <c r="A1029" s="6"/>
-      <c r="B1029" s="6"/>
-      <c r="C1029" s="6"/>
-      <c r="D1029" s="7"/>
-      <c r="E1029" s="7"/>
+      <c r="A1029" s="1"/>
+      <c r="B1029" s="1"/>
+      <c r="C1029" s="1"/>
+      <c r="D1029" s="2"/>
+      <c r="E1029" s="2"/>
       <c r="F1029" s="3"/>
       <c r="G1029" s="3"/>
       <c r="H1029" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1030" customHeight="1" ht="19.5">
-      <c r="A1030" s="6"/>
-      <c r="B1030" s="6"/>
-      <c r="C1030" s="6"/>
-      <c r="D1030" s="7"/>
-      <c r="E1030" s="7"/>
+      <c r="A1030" s="1"/>
+      <c r="B1030" s="1"/>
+      <c r="C1030" s="1"/>
+      <c r="D1030" s="2"/>
+      <c r="E1030" s="2"/>
       <c r="F1030" s="3"/>
       <c r="G1030" s="3"/>
       <c r="H1030" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1031" customHeight="1" ht="19.5">
-      <c r="A1031" s="6"/>
-      <c r="B1031" s="6"/>
-      <c r="C1031" s="6"/>
-      <c r="D1031" s="7"/>
-      <c r="E1031" s="7"/>
+      <c r="A1031" s="1"/>
+      <c r="B1031" s="1"/>
+      <c r="C1031" s="1"/>
+      <c r="D1031" s="2"/>
+      <c r="E1031" s="2"/>
       <c r="F1031" s="3"/>
       <c r="G1031" s="3"/>
       <c r="H1031" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1032" customHeight="1" ht="19.5">
-      <c r="A1032" s="6"/>
-      <c r="B1032" s="6"/>
-      <c r="C1032" s="6"/>
-      <c r="D1032" s="7"/>
-      <c r="E1032" s="7"/>
+      <c r="A1032" s="1"/>
+      <c r="B1032" s="1"/>
+      <c r="C1032" s="1"/>
+      <c r="D1032" s="2"/>
+      <c r="E1032" s="2"/>
       <c r="F1032" s="3"/>
       <c r="G1032" s="3"/>
       <c r="H1032" s="3"/>
@@ -28262,8 +28307,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1105" customHeight="1" ht="19.5">
       <c r="A1105" s="1"/>
-      <c r="B1105" s="2"/>
-      <c r="C1105" s="2"/>
+      <c r="B1105" s="1"/>
+      <c r="C1105" s="1"/>
       <c r="D1105" s="2"/>
       <c r="E1105" s="2"/>
       <c r="F1105" s="3"/>
@@ -28312,8 +28357,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1110" customHeight="1" ht="19.5">
       <c r="A1110" s="1"/>
-      <c r="B1110" s="1"/>
-      <c r="C1110" s="1"/>
+      <c r="B1110" s="2"/>
+      <c r="C1110" s="2"/>
       <c r="D1110" s="2"/>
       <c r="E1110" s="2"/>
       <c r="F1110" s="3"/>
@@ -28392,7 +28437,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1118" customHeight="1" ht="19.5">
       <c r="A1118" s="1"/>
-      <c r="B1118" s="2"/>
+      <c r="B1118" s="1"/>
       <c r="C1118" s="1"/>
       <c r="D1118" s="2"/>
       <c r="E1118" s="2"/>
@@ -28422,8 +28467,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1121" customHeight="1" ht="19.5">
       <c r="A1121" s="1"/>
-      <c r="B1121" s="2"/>
-      <c r="C1121" s="2"/>
+      <c r="B1121" s="1"/>
+      <c r="C1121" s="1"/>
       <c r="D1121" s="2"/>
       <c r="E1121" s="2"/>
       <c r="F1121" s="3"/>
@@ -28432,8 +28477,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1122" customHeight="1" ht="19.5">
       <c r="A1122" s="1"/>
-      <c r="B1122" s="2"/>
-      <c r="C1122" s="2"/>
+      <c r="B1122" s="1"/>
+      <c r="C1122" s="1"/>
       <c r="D1122" s="2"/>
       <c r="E1122" s="2"/>
       <c r="F1122" s="3"/>
@@ -28442,7 +28487,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1123" customHeight="1" ht="19.5">
       <c r="A1123" s="1"/>
-      <c r="B1123" s="1"/>
+      <c r="B1123" s="2"/>
       <c r="C1123" s="1"/>
       <c r="D1123" s="2"/>
       <c r="E1123" s="2"/>
@@ -28462,7 +28507,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1125" customHeight="1" ht="19.5">
       <c r="A1125" s="1"/>
-      <c r="B1125" s="2"/>
+      <c r="B1125" s="1"/>
       <c r="C1125" s="1"/>
       <c r="D1125" s="2"/>
       <c r="E1125" s="2"/>
@@ -28472,8 +28517,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1126" customHeight="1" ht="19.5">
       <c r="A1126" s="1"/>
-      <c r="B1126" s="1"/>
-      <c r="C1126" s="1"/>
+      <c r="B1126" s="2"/>
+      <c r="C1126" s="2"/>
       <c r="D1126" s="2"/>
       <c r="E1126" s="2"/>
       <c r="F1126" s="3"/>
@@ -28482,8 +28527,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1127" customHeight="1" ht="19.5">
       <c r="A1127" s="1"/>
-      <c r="B1127" s="1"/>
-      <c r="C1127" s="1"/>
+      <c r="B1127" s="2"/>
+      <c r="C1127" s="2"/>
       <c r="D1127" s="2"/>
       <c r="E1127" s="2"/>
       <c r="F1127" s="3"/>
@@ -28492,8 +28537,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1128" customHeight="1" ht="19.5">
       <c r="A1128" s="1"/>
-      <c r="B1128" s="2"/>
-      <c r="C1128" s="2"/>
+      <c r="B1128" s="1"/>
+      <c r="C1128" s="1"/>
       <c r="D1128" s="2"/>
       <c r="E1128" s="2"/>
       <c r="F1128" s="3"/>
@@ -28502,8 +28547,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1129" customHeight="1" ht="19.5">
       <c r="A1129" s="1"/>
-      <c r="B1129" s="2"/>
-      <c r="C1129" s="2"/>
+      <c r="B1129" s="1"/>
+      <c r="C1129" s="1"/>
       <c r="D1129" s="2"/>
       <c r="E1129" s="2"/>
       <c r="F1129" s="3"/>
@@ -28531,29 +28576,29 @@
       <c r="H1131" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1132" customHeight="1" ht="19.5">
-      <c r="A1132" s="6"/>
-      <c r="B1132" s="6"/>
-      <c r="C1132" s="6"/>
-      <c r="D1132" s="7"/>
-      <c r="E1132" s="7"/>
+      <c r="A1132" s="1"/>
+      <c r="B1132" s="1"/>
+      <c r="C1132" s="1"/>
+      <c r="D1132" s="2"/>
+      <c r="E1132" s="2"/>
       <c r="F1132" s="3"/>
       <c r="G1132" s="3"/>
       <c r="H1132" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1133" customHeight="1" ht="19.5">
-      <c r="A1133" s="6"/>
-      <c r="B1133" s="6"/>
-      <c r="C1133" s="6"/>
-      <c r="D1133" s="7"/>
-      <c r="E1133" s="7"/>
+      <c r="A1133" s="1"/>
+      <c r="B1133" s="2"/>
+      <c r="C1133" s="2"/>
+      <c r="D1133" s="2"/>
+      <c r="E1133" s="2"/>
       <c r="F1133" s="3"/>
       <c r="G1133" s="3"/>
       <c r="H1133" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1134" customHeight="1" ht="19.5">
       <c r="A1134" s="1"/>
-      <c r="B1134" s="1"/>
-      <c r="C1134" s="1"/>
+      <c r="B1134" s="2"/>
+      <c r="C1134" s="2"/>
       <c r="D1134" s="2"/>
       <c r="E1134" s="2"/>
       <c r="F1134" s="3"/>
@@ -28572,7 +28617,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1136" customHeight="1" ht="19.5">
       <c r="A1136" s="1"/>
-      <c r="B1136" s="2"/>
+      <c r="B1136" s="1"/>
       <c r="C1136" s="1"/>
       <c r="D1136" s="2"/>
       <c r="E1136" s="2"/>
@@ -28592,7 +28637,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1138" customHeight="1" ht="19.5">
       <c r="A1138" s="1"/>
-      <c r="B1138" s="2"/>
+      <c r="B1138" s="1"/>
       <c r="C1138" s="1"/>
       <c r="D1138" s="2"/>
       <c r="E1138" s="2"/>
@@ -28632,7 +28677,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1142" customHeight="1" ht="19.5">
       <c r="A1142" s="1"/>
-      <c r="B1142" s="2"/>
+      <c r="B1142" s="1"/>
       <c r="C1142" s="1"/>
       <c r="D1142" s="2"/>
       <c r="E1142" s="2"/>
@@ -28652,7 +28697,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1144" customHeight="1" ht="19.5">
       <c r="A1144" s="1"/>
-      <c r="B1144" s="2"/>
+      <c r="B1144" s="1"/>
       <c r="C1144" s="1"/>
       <c r="D1144" s="2"/>
       <c r="E1144" s="2"/>
@@ -28702,7 +28747,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1149" customHeight="1" ht="19.5">
       <c r="A1149" s="1"/>
-      <c r="B1149" s="1"/>
+      <c r="B1149" s="2"/>
       <c r="C1149" s="1"/>
       <c r="D1149" s="2"/>
       <c r="E1149" s="2"/>
@@ -28712,7 +28757,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1150" customHeight="1" ht="19.5">
       <c r="A1150" s="1"/>
-      <c r="B1150" s="1"/>
+      <c r="B1150" s="2"/>
       <c r="C1150" s="1"/>
       <c r="D1150" s="2"/>
       <c r="E1150" s="2"/>
@@ -28722,7 +28767,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1151" customHeight="1" ht="19.5">
       <c r="A1151" s="1"/>
-      <c r="B1151" s="1"/>
+      <c r="B1151" s="2"/>
       <c r="C1151" s="1"/>
       <c r="D1151" s="2"/>
       <c r="E1151" s="2"/>
@@ -28732,7 +28777,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1152" customHeight="1" ht="19.5">
       <c r="A1152" s="1"/>
-      <c r="B1152" s="1"/>
+      <c r="B1152" s="2"/>
       <c r="C1152" s="1"/>
       <c r="D1152" s="2"/>
       <c r="E1152" s="2"/>
@@ -28742,7 +28787,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1153" customHeight="1" ht="19.5">
       <c r="A1153" s="1"/>
-      <c r="B1153" s="1"/>
+      <c r="B1153" s="2"/>
       <c r="C1153" s="1"/>
       <c r="D1153" s="2"/>
       <c r="E1153" s="2"/>
@@ -29082,8 +29127,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1187" customHeight="1" ht="19.5">
       <c r="A1187" s="1"/>
-      <c r="B1187" s="2"/>
-      <c r="C1187" s="2"/>
+      <c r="B1187" s="1"/>
+      <c r="C1187" s="1"/>
       <c r="D1187" s="2"/>
       <c r="E1187" s="2"/>
       <c r="F1187" s="3"/>
@@ -29112,8 +29157,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1190" customHeight="1" ht="19.5">
       <c r="A1190" s="1"/>
-      <c r="B1190" s="2"/>
-      <c r="C1190" s="2"/>
+      <c r="B1190" s="1"/>
+      <c r="C1190" s="1"/>
       <c r="D1190" s="2"/>
       <c r="E1190" s="2"/>
       <c r="F1190" s="3"/>
@@ -29122,8 +29167,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1191" customHeight="1" ht="19.5">
       <c r="A1191" s="1"/>
-      <c r="B1191" s="2"/>
-      <c r="C1191" s="2"/>
+      <c r="B1191" s="1"/>
+      <c r="C1191" s="1"/>
       <c r="D1191" s="2"/>
       <c r="E1191" s="2"/>
       <c r="F1191" s="3"/>
@@ -29152,8 +29197,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1194" customHeight="1" ht="19.5">
       <c r="A1194" s="1"/>
-      <c r="B1194" s="2"/>
-      <c r="C1194" s="2"/>
+      <c r="B1194" s="1"/>
+      <c r="C1194" s="1"/>
       <c r="D1194" s="2"/>
       <c r="E1194" s="2"/>
       <c r="F1194" s="3"/>
@@ -29162,8 +29207,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1195" customHeight="1" ht="19.5">
       <c r="A1195" s="1"/>
-      <c r="B1195" s="1"/>
-      <c r="C1195" s="1"/>
+      <c r="B1195" s="2"/>
+      <c r="C1195" s="2"/>
       <c r="D1195" s="2"/>
       <c r="E1195" s="2"/>
       <c r="F1195" s="3"/>
@@ -29172,8 +29217,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1196" customHeight="1" ht="19.5">
       <c r="A1196" s="1"/>
-      <c r="B1196" s="1"/>
-      <c r="C1196" s="1"/>
+      <c r="B1196" s="2"/>
+      <c r="C1196" s="2"/>
       <c r="D1196" s="2"/>
       <c r="E1196" s="2"/>
       <c r="F1196" s="3"/>
@@ -29183,7 +29228,7 @@
     <row x14ac:dyDescent="0.25" r="1197" customHeight="1" ht="19.5">
       <c r="A1197" s="1"/>
       <c r="B1197" s="2"/>
-      <c r="C1197" s="1"/>
+      <c r="C1197" s="2"/>
       <c r="D1197" s="2"/>
       <c r="E1197" s="2"/>
       <c r="F1197" s="3"/>
@@ -29202,8 +29247,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1199" customHeight="1" ht="19.5">
       <c r="A1199" s="1"/>
-      <c r="B1199" s="1"/>
-      <c r="C1199" s="1"/>
+      <c r="B1199" s="2"/>
+      <c r="C1199" s="2"/>
       <c r="D1199" s="2"/>
       <c r="E1199" s="2"/>
       <c r="F1199" s="3"/>
@@ -29232,7 +29277,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1202" customHeight="1" ht="19.5">
       <c r="A1202" s="1"/>
-      <c r="B1202" s="1"/>
+      <c r="B1202" s="2"/>
       <c r="C1202" s="1"/>
       <c r="D1202" s="2"/>
       <c r="E1202" s="2"/>
@@ -29252,7 +29297,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1204" customHeight="1" ht="19.5">
       <c r="A1204" s="1"/>
-      <c r="B1204" s="2"/>
+      <c r="B1204" s="1"/>
       <c r="C1204" s="1"/>
       <c r="D1204" s="2"/>
       <c r="E1204" s="2"/>
@@ -29272,7 +29317,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1206" customHeight="1" ht="19.5">
       <c r="A1206" s="1"/>
-      <c r="B1206" s="2"/>
+      <c r="B1206" s="1"/>
       <c r="C1206" s="1"/>
       <c r="D1206" s="2"/>
       <c r="E1206" s="2"/>
@@ -29302,7 +29347,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1209" customHeight="1" ht="19.5">
       <c r="A1209" s="1"/>
-      <c r="B1209" s="1"/>
+      <c r="B1209" s="2"/>
       <c r="C1209" s="1"/>
       <c r="D1209" s="2"/>
       <c r="E1209" s="2"/>
@@ -29322,7 +29367,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1211" customHeight="1" ht="19.5">
       <c r="A1211" s="1"/>
-      <c r="B1211" s="1"/>
+      <c r="B1211" s="2"/>
       <c r="C1211" s="1"/>
       <c r="D1211" s="2"/>
       <c r="E1211" s="2"/>
@@ -29382,8 +29427,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1217" customHeight="1" ht="19.5">
       <c r="A1217" s="1"/>
-      <c r="B1217" s="2"/>
-      <c r="C1217" s="2"/>
+      <c r="B1217" s="1"/>
+      <c r="C1217" s="1"/>
       <c r="D1217" s="2"/>
       <c r="E1217" s="2"/>
       <c r="F1217" s="3"/>
@@ -29392,8 +29437,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1218" customHeight="1" ht="19.5">
       <c r="A1218" s="1"/>
-      <c r="B1218" s="2"/>
-      <c r="C1218" s="2"/>
+      <c r="B1218" s="1"/>
+      <c r="C1218" s="1"/>
       <c r="D1218" s="2"/>
       <c r="E1218" s="2"/>
       <c r="F1218" s="3"/>
@@ -29432,8 +29477,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1222" customHeight="1" ht="19.5">
       <c r="A1222" s="1"/>
-      <c r="B1222" s="1"/>
-      <c r="C1222" s="1"/>
+      <c r="B1222" s="2"/>
+      <c r="C1222" s="2"/>
       <c r="D1222" s="2"/>
       <c r="E1222" s="2"/>
       <c r="F1222" s="3"/>
@@ -29442,8 +29487,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1223" customHeight="1" ht="19.5">
       <c r="A1223" s="1"/>
-      <c r="B1223" s="1"/>
-      <c r="C1223" s="1"/>
+      <c r="B1223" s="2"/>
+      <c r="C1223" s="2"/>
       <c r="D1223" s="2"/>
       <c r="E1223" s="2"/>
       <c r="F1223" s="3"/>
@@ -29462,8 +29507,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1225" customHeight="1" ht="19.5">
       <c r="A1225" s="1"/>
-      <c r="B1225" s="2"/>
-      <c r="C1225" s="2"/>
+      <c r="B1225" s="1"/>
+      <c r="C1225" s="1"/>
       <c r="D1225" s="2"/>
       <c r="E1225" s="2"/>
       <c r="F1225" s="3"/>
@@ -29472,8 +29517,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1226" customHeight="1" ht="19.5">
       <c r="A1226" s="1"/>
-      <c r="B1226" s="2"/>
-      <c r="C1226" s="2"/>
+      <c r="B1226" s="1"/>
+      <c r="C1226" s="1"/>
       <c r="D1226" s="2"/>
       <c r="E1226" s="2"/>
       <c r="F1226" s="3"/>
@@ -29492,8 +29537,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1228" customHeight="1" ht="19.5">
       <c r="A1228" s="1"/>
-      <c r="B1228" s="2"/>
-      <c r="C1228" s="2"/>
+      <c r="B1228" s="1"/>
+      <c r="C1228" s="1"/>
       <c r="D1228" s="2"/>
       <c r="E1228" s="2"/>
       <c r="F1228" s="3"/>
@@ -29502,8 +29547,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1229" customHeight="1" ht="19.5">
       <c r="A1229" s="1"/>
-      <c r="B1229" s="2"/>
-      <c r="C1229" s="2"/>
+      <c r="B1229" s="1"/>
+      <c r="C1229" s="1"/>
       <c r="D1229" s="2"/>
       <c r="E1229" s="2"/>
       <c r="F1229" s="3"/>
@@ -29522,8 +29567,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1231" customHeight="1" ht="19.5">
       <c r="A1231" s="1"/>
-      <c r="B1231" s="1"/>
-      <c r="C1231" s="1"/>
+      <c r="B1231" s="2"/>
+      <c r="C1231" s="2"/>
       <c r="D1231" s="2"/>
       <c r="E1231" s="2"/>
       <c r="F1231" s="3"/>
@@ -29542,8 +29587,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1233" customHeight="1" ht="19.5">
       <c r="A1233" s="1"/>
-      <c r="B1233" s="1"/>
-      <c r="C1233" s="1"/>
+      <c r="B1233" s="2"/>
+      <c r="C1233" s="2"/>
       <c r="D1233" s="2"/>
       <c r="E1233" s="2"/>
       <c r="F1233" s="3"/>
@@ -29573,7 +29618,7 @@
     <row x14ac:dyDescent="0.25" r="1236" customHeight="1" ht="19.5">
       <c r="A1236" s="1"/>
       <c r="B1236" s="1"/>
-      <c r="C1236" s="2"/>
+      <c r="C1236" s="1"/>
       <c r="D1236" s="2"/>
       <c r="E1236" s="2"/>
       <c r="F1236" s="3"/>
@@ -29602,8 +29647,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1239" customHeight="1" ht="19.5">
       <c r="A1239" s="1"/>
-      <c r="B1239" s="1"/>
-      <c r="C1239" s="1"/>
+      <c r="B1239" s="2"/>
+      <c r="C1239" s="2"/>
       <c r="D1239" s="2"/>
       <c r="E1239" s="2"/>
       <c r="F1239" s="3"/>
@@ -29612,8 +29657,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1240" customHeight="1" ht="19.5">
       <c r="A1240" s="1"/>
-      <c r="B1240" s="1"/>
-      <c r="C1240" s="1"/>
+      <c r="B1240" s="2"/>
+      <c r="C1240" s="2"/>
       <c r="D1240" s="2"/>
       <c r="E1240" s="2"/>
       <c r="F1240" s="3"/>
@@ -29623,7 +29668,7 @@
     <row x14ac:dyDescent="0.25" r="1241" customHeight="1" ht="19.5">
       <c r="A1241" s="1"/>
       <c r="B1241" s="1"/>
-      <c r="C1241" s="1"/>
+      <c r="C1241" s="2"/>
       <c r="D1241" s="2"/>
       <c r="E1241" s="2"/>
       <c r="F1241" s="3"/>
@@ -29792,7 +29837,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1258" customHeight="1" ht="19.5">
       <c r="A1258" s="1"/>
-      <c r="B1258" s="2"/>
+      <c r="B1258" s="1"/>
       <c r="C1258" s="1"/>
       <c r="D1258" s="2"/>
       <c r="E1258" s="2"/>
@@ -29842,7 +29887,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1263" customHeight="1" ht="19.5">
       <c r="A1263" s="1"/>
-      <c r="B1263" s="1"/>
+      <c r="B1263" s="2"/>
       <c r="C1263" s="1"/>
       <c r="D1263" s="2"/>
       <c r="E1263" s="2"/>
@@ -29862,8 +29907,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1265" customHeight="1" ht="19.5">
       <c r="A1265" s="1"/>
-      <c r="B1265" s="2"/>
-      <c r="C1265" s="2"/>
+      <c r="B1265" s="1"/>
+      <c r="C1265" s="1"/>
       <c r="D1265" s="2"/>
       <c r="E1265" s="2"/>
       <c r="F1265" s="3"/>
@@ -29882,8 +29927,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1267" customHeight="1" ht="19.5">
       <c r="A1267" s="1"/>
-      <c r="B1267" s="2"/>
-      <c r="C1267" s="2"/>
+      <c r="B1267" s="1"/>
+      <c r="C1267" s="1"/>
       <c r="D1267" s="2"/>
       <c r="E1267" s="2"/>
       <c r="F1267" s="3"/>
@@ -29912,7 +29957,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1270" customHeight="1" ht="19.5">
       <c r="A1270" s="1"/>
-      <c r="B1270" s="1"/>
+      <c r="B1270" s="2"/>
       <c r="C1270" s="2"/>
       <c r="D1270" s="2"/>
       <c r="E1270" s="2"/>
@@ -29922,8 +29967,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1271" customHeight="1" ht="19.5">
       <c r="A1271" s="1"/>
-      <c r="B1271" s="2"/>
-      <c r="C1271" s="2"/>
+      <c r="B1271" s="1"/>
+      <c r="C1271" s="1"/>
       <c r="D1271" s="2"/>
       <c r="E1271" s="2"/>
       <c r="F1271" s="3"/>
@@ -29932,8 +29977,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1272" customHeight="1" ht="19.5">
       <c r="A1272" s="1"/>
-      <c r="B1272" s="1"/>
-      <c r="C1272" s="1"/>
+      <c r="B1272" s="2"/>
+      <c r="C1272" s="2"/>
       <c r="D1272" s="2"/>
       <c r="E1272" s="2"/>
       <c r="F1272" s="3"/>
@@ -29963,7 +30008,7 @@
     <row x14ac:dyDescent="0.25" r="1275" customHeight="1" ht="19.5">
       <c r="A1275" s="1"/>
       <c r="B1275" s="1"/>
-      <c r="C1275" s="1"/>
+      <c r="C1275" s="2"/>
       <c r="D1275" s="2"/>
       <c r="E1275" s="2"/>
       <c r="F1275" s="3"/>
@@ -29972,8 +30017,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1276" customHeight="1" ht="19.5">
       <c r="A1276" s="1"/>
-      <c r="B1276" s="1"/>
-      <c r="C1276" s="1"/>
+      <c r="B1276" s="2"/>
+      <c r="C1276" s="2"/>
       <c r="D1276" s="2"/>
       <c r="E1276" s="2"/>
       <c r="F1276" s="3"/>
@@ -29993,7 +30038,7 @@
     <row x14ac:dyDescent="0.25" r="1278" customHeight="1" ht="19.5">
       <c r="A1278" s="1"/>
       <c r="B1278" s="1"/>
-      <c r="C1278" s="2"/>
+      <c r="C1278" s="1"/>
       <c r="D1278" s="2"/>
       <c r="E1278" s="2"/>
       <c r="F1278" s="3"/>
@@ -30003,7 +30048,7 @@
     <row x14ac:dyDescent="0.25" r="1279" customHeight="1" ht="19.5">
       <c r="A1279" s="1"/>
       <c r="B1279" s="1"/>
-      <c r="C1279" s="2"/>
+      <c r="C1279" s="1"/>
       <c r="D1279" s="2"/>
       <c r="E1279" s="2"/>
       <c r="F1279" s="3"/>
@@ -30012,8 +30057,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1280" customHeight="1" ht="19.5">
       <c r="A1280" s="1"/>
-      <c r="B1280" s="2"/>
-      <c r="C1280" s="2"/>
+      <c r="B1280" s="1"/>
+      <c r="C1280" s="1"/>
       <c r="D1280" s="2"/>
       <c r="E1280" s="2"/>
       <c r="F1280" s="3"/>
@@ -30022,8 +30067,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1281" customHeight="1" ht="19.5">
       <c r="A1281" s="1"/>
-      <c r="B1281" s="2"/>
-      <c r="C1281" s="2"/>
+      <c r="B1281" s="1"/>
+      <c r="C1281" s="1"/>
       <c r="D1281" s="2"/>
       <c r="E1281" s="2"/>
       <c r="F1281" s="3"/>
@@ -30032,8 +30077,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1282" customHeight="1" ht="19.5">
       <c r="A1282" s="1"/>
-      <c r="B1282" s="2"/>
-      <c r="C1282" s="2"/>
+      <c r="B1282" s="1"/>
+      <c r="C1282" s="1"/>
       <c r="D1282" s="2"/>
       <c r="E1282" s="2"/>
       <c r="F1282" s="3"/>
@@ -30043,7 +30088,7 @@
     <row x14ac:dyDescent="0.25" r="1283" customHeight="1" ht="19.5">
       <c r="A1283" s="1"/>
       <c r="B1283" s="1"/>
-      <c r="C1283" s="1"/>
+      <c r="C1283" s="2"/>
       <c r="D1283" s="2"/>
       <c r="E1283" s="2"/>
       <c r="F1283" s="3"/>
@@ -30053,7 +30098,7 @@
     <row x14ac:dyDescent="0.25" r="1284" customHeight="1" ht="19.5">
       <c r="A1284" s="1"/>
       <c r="B1284" s="1"/>
-      <c r="C1284" s="1"/>
+      <c r="C1284" s="2"/>
       <c r="D1284" s="2"/>
       <c r="E1284" s="2"/>
       <c r="F1284" s="3"/>
@@ -30062,8 +30107,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1285" customHeight="1" ht="19.5">
       <c r="A1285" s="1"/>
-      <c r="B1285" s="1"/>
-      <c r="C1285" s="1"/>
+      <c r="B1285" s="2"/>
+      <c r="C1285" s="2"/>
       <c r="D1285" s="2"/>
       <c r="E1285" s="2"/>
       <c r="F1285" s="3"/>
@@ -30072,8 +30117,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1286" customHeight="1" ht="19.5">
       <c r="A1286" s="1"/>
-      <c r="B1286" s="1"/>
-      <c r="C1286" s="1"/>
+      <c r="B1286" s="2"/>
+      <c r="C1286" s="2"/>
       <c r="D1286" s="2"/>
       <c r="E1286" s="2"/>
       <c r="F1286" s="3"/>
@@ -30082,8 +30127,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1287" customHeight="1" ht="19.5">
       <c r="A1287" s="1"/>
-      <c r="B1287" s="1"/>
-      <c r="C1287" s="1"/>
+      <c r="B1287" s="2"/>
+      <c r="C1287" s="2"/>
       <c r="D1287" s="2"/>
       <c r="E1287" s="2"/>
       <c r="F1287" s="3"/>
@@ -30092,8 +30137,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1288" customHeight="1" ht="19.5">
       <c r="A1288" s="1"/>
-      <c r="B1288" s="2"/>
-      <c r="C1288" s="2"/>
+      <c r="B1288" s="1"/>
+      <c r="C1288" s="1"/>
       <c r="D1288" s="2"/>
       <c r="E1288" s="2"/>
       <c r="F1288" s="3"/>
@@ -30142,8 +30187,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1293" customHeight="1" ht="19.5">
       <c r="A1293" s="1"/>
-      <c r="B1293" s="1"/>
-      <c r="C1293" s="1"/>
+      <c r="B1293" s="2"/>
+      <c r="C1293" s="2"/>
       <c r="D1293" s="2"/>
       <c r="E1293" s="2"/>
       <c r="F1293" s="3"/>
@@ -30152,8 +30197,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1294" customHeight="1" ht="19.5">
       <c r="A1294" s="1"/>
-      <c r="B1294" s="2"/>
-      <c r="C1294" s="2"/>
+      <c r="B1294" s="1"/>
+      <c r="C1294" s="1"/>
       <c r="D1294" s="2"/>
       <c r="E1294" s="2"/>
       <c r="F1294" s="3"/>
@@ -30163,7 +30208,7 @@
     <row x14ac:dyDescent="0.25" r="1295" customHeight="1" ht="19.5">
       <c r="A1295" s="1"/>
       <c r="B1295" s="1"/>
-      <c r="C1295" s="2"/>
+      <c r="C1295" s="1"/>
       <c r="D1295" s="2"/>
       <c r="E1295" s="2"/>
       <c r="F1295" s="3"/>
@@ -30172,8 +30217,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1296" customHeight="1" ht="19.5">
       <c r="A1296" s="1"/>
-      <c r="B1296" s="2"/>
-      <c r="C1296" s="2"/>
+      <c r="B1296" s="1"/>
+      <c r="C1296" s="1"/>
       <c r="D1296" s="2"/>
       <c r="E1296" s="2"/>
       <c r="F1296" s="3"/>
@@ -30182,7 +30227,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1297" customHeight="1" ht="19.5">
       <c r="A1297" s="1"/>
-      <c r="B1297" s="2"/>
+      <c r="B1297" s="1"/>
       <c r="C1297" s="1"/>
       <c r="D1297" s="2"/>
       <c r="E1297" s="2"/>
@@ -30192,8 +30237,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1298" customHeight="1" ht="19.5">
       <c r="A1298" s="1"/>
-      <c r="B1298" s="2"/>
-      <c r="C1298" s="2"/>
+      <c r="B1298" s="1"/>
+      <c r="C1298" s="1"/>
       <c r="D1298" s="2"/>
       <c r="E1298" s="2"/>
       <c r="F1298" s="3"/>
@@ -30213,7 +30258,7 @@
     <row x14ac:dyDescent="0.25" r="1300" customHeight="1" ht="19.5">
       <c r="A1300" s="1"/>
       <c r="B1300" s="1"/>
-      <c r="C1300" s="1"/>
+      <c r="C1300" s="2"/>
       <c r="D1300" s="2"/>
       <c r="E1300" s="2"/>
       <c r="F1300" s="3"/>
@@ -30222,8 +30267,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1301" customHeight="1" ht="19.5">
       <c r="A1301" s="1"/>
-      <c r="B1301" s="1"/>
-      <c r="C1301" s="1"/>
+      <c r="B1301" s="2"/>
+      <c r="C1301" s="2"/>
       <c r="D1301" s="2"/>
       <c r="E1301" s="2"/>
       <c r="F1301" s="3"/>
@@ -30232,7 +30277,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1302" customHeight="1" ht="19.5">
       <c r="A1302" s="1"/>
-      <c r="B1302" s="1"/>
+      <c r="B1302" s="2"/>
       <c r="C1302" s="1"/>
       <c r="D1302" s="2"/>
       <c r="E1302" s="2"/>
@@ -30292,7 +30337,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1308" customHeight="1" ht="19.5">
       <c r="A1308" s="1"/>
-      <c r="B1308" s="1"/>
+      <c r="B1308" s="2"/>
       <c r="C1308" s="2"/>
       <c r="D1308" s="2"/>
       <c r="E1308" s="2"/>
@@ -30302,8 +30347,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1309" customHeight="1" ht="19.5">
       <c r="A1309" s="1"/>
-      <c r="B1309" s="1"/>
-      <c r="C1309" s="1"/>
+      <c r="B1309" s="2"/>
+      <c r="C1309" s="2"/>
       <c r="D1309" s="2"/>
       <c r="E1309" s="2"/>
       <c r="F1309" s="3"/>
@@ -30342,7 +30387,7 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1313" customHeight="1" ht="19.5">
       <c r="A1313" s="1"/>
-      <c r="B1313" s="2"/>
+      <c r="B1313" s="1"/>
       <c r="C1313" s="2"/>
       <c r="D1313" s="2"/>
       <c r="E1313" s="2"/>
@@ -30362,8 +30407,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1315" customHeight="1" ht="19.5">
       <c r="A1315" s="1"/>
-      <c r="B1315" s="2"/>
-      <c r="C1315" s="2"/>
+      <c r="B1315" s="1"/>
+      <c r="C1315" s="1"/>
       <c r="D1315" s="2"/>
       <c r="E1315" s="2"/>
       <c r="F1315" s="3"/>
@@ -30372,8 +30417,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1316" customHeight="1" ht="19.5">
       <c r="A1316" s="1"/>
-      <c r="B1316" s="2"/>
-      <c r="C1316" s="2"/>
+      <c r="B1316" s="1"/>
+      <c r="C1316" s="1"/>
       <c r="D1316" s="2"/>
       <c r="E1316" s="2"/>
       <c r="F1316" s="3"/>
@@ -30382,8 +30427,8 @@
     </row>
     <row x14ac:dyDescent="0.25" r="1317" customHeight="1" ht="19.5">
       <c r="A1317" s="1"/>
-      <c r="B1317" s="2"/>
-      <c r="C1317" s="2"/>
+      <c r="B1317" s="1"/>
+      <c r="C1317" s="1"/>
       <c r="D1317" s="2"/>
       <c r="E1317" s="2"/>
       <c r="F1317" s="3"/>
@@ -30399,6 +30444,56 @@
       <c r="F1318" s="3"/>
       <c r="G1318" s="3"/>
       <c r="H1318" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1319" customHeight="1" ht="19.5">
+      <c r="A1319" s="1"/>
+      <c r="B1319" s="1"/>
+      <c r="C1319" s="1"/>
+      <c r="D1319" s="2"/>
+      <c r="E1319" s="2"/>
+      <c r="F1319" s="3"/>
+      <c r="G1319" s="3"/>
+      <c r="H1319" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1320" customHeight="1" ht="19.5">
+      <c r="A1320" s="1"/>
+      <c r="B1320" s="2"/>
+      <c r="C1320" s="2"/>
+      <c r="D1320" s="2"/>
+      <c r="E1320" s="2"/>
+      <c r="F1320" s="3"/>
+      <c r="G1320" s="3"/>
+      <c r="H1320" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1321" customHeight="1" ht="19.5">
+      <c r="A1321" s="1"/>
+      <c r="B1321" s="2"/>
+      <c r="C1321" s="2"/>
+      <c r="D1321" s="2"/>
+      <c r="E1321" s="2"/>
+      <c r="F1321" s="3"/>
+      <c r="G1321" s="3"/>
+      <c r="H1321" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1322" customHeight="1" ht="19.5">
+      <c r="A1322" s="1"/>
+      <c r="B1322" s="2"/>
+      <c r="C1322" s="2"/>
+      <c r="D1322" s="2"/>
+      <c r="E1322" s="2"/>
+      <c r="F1322" s="3"/>
+      <c r="G1322" s="3"/>
+      <c r="H1322" s="3"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="1323" customHeight="1" ht="19.5">
+      <c r="A1323" s="1"/>
+      <c r="B1323" s="2"/>
+      <c r="C1323" s="2"/>
+      <c r="D1323" s="2"/>
+      <c r="E1323" s="2"/>
+      <c r="F1323" s="3"/>
+      <c r="G1323" s="3"/>
+      <c r="H1323" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -30416,14 +30511,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="11" width="45.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="49.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="11" width="49.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="12" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="12" width="33.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="9" width="45.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="9" width="49.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="49.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="10" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="10" width="33.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -37265,11 +37360,11 @@
       <c r="H433" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="434" customHeight="1" ht="19.5">
-      <c r="A434" s="6"/>
-      <c r="B434" s="6"/>
-      <c r="C434" s="6"/>
-      <c r="D434" s="7"/>
-      <c r="E434" s="7"/>
+      <c r="A434" s="1"/>
+      <c r="B434" s="1"/>
+      <c r="C434" s="1"/>
+      <c r="D434" s="2"/>
+      <c r="E434" s="2"/>
       <c r="F434" s="3"/>
       <c r="G434" s="3"/>
       <c r="H434" s="3"/>
@@ -37364,7 +37459,7 @@
       <c r="G440" s="3"/>
       <c r="H440" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="19.5" customFormat="1" s="8">
+    <row x14ac:dyDescent="0.25" r="441" customHeight="1" ht="19.5" customFormat="1" s="6">
       <c r="A441" s="2"/>
       <c r="B441" s="2"/>
       <c r="C441" s="2"/>
@@ -37874,7 +37969,7 @@
       <c r="A473" s="1" t="s">
         <v>1188</v>
       </c>
-      <c r="B473" s="9" t="s">
+      <c r="B473" s="7" t="s">
         <v>1189</v>
       </c>
       <c r="C473" s="1" t="s">
@@ -37890,7 +37985,7 @@
       <c r="A474" s="1" t="s">
         <v>1191</v>
       </c>
-      <c r="B474" s="9" t="s">
+      <c r="B474" s="7" t="s">
         <v>1192</v>
       </c>
       <c r="C474" s="1" t="s">
@@ -37938,7 +38033,7 @@
       <c r="A477" s="1" t="s">
         <v>1198</v>
       </c>
-      <c r="B477" s="9" t="s">
+      <c r="B477" s="7" t="s">
         <v>1199</v>
       </c>
       <c r="C477" s="1" t="s">
@@ -37970,7 +38065,7 @@
       <c r="A479" s="1" t="s">
         <v>1203</v>
       </c>
-      <c r="B479" s="9" t="s">
+      <c r="B479" s="7" t="s">
         <v>1204</v>
       </c>
       <c r="C479" s="1" t="s">
@@ -38268,8 +38363,8 @@
       <c r="C498" s="1" t="s">
         <v>1245</v>
       </c>
-      <c r="D498" s="7"/>
-      <c r="E498" s="7"/>
+      <c r="D498" s="2"/>
+      <c r="E498" s="2"/>
       <c r="F498" s="3"/>
       <c r="G498" s="3"/>
       <c r="H498" s="3"/>
@@ -39010,7 +39105,7 @@
       <c r="A545" s="1" t="s">
         <v>1368</v>
       </c>
-      <c r="B545" s="9" t="s">
+      <c r="B545" s="7" t="s">
         <v>1369</v>
       </c>
       <c r="C545" s="1" t="s">
@@ -39026,7 +39121,7 @@
       <c r="A546" s="1" t="s">
         <v>1371</v>
       </c>
-      <c r="B546" s="9" t="s">
+      <c r="B546" s="7" t="s">
         <v>1372</v>
       </c>
       <c r="C546" s="2" t="s">
@@ -39086,7 +39181,7 @@
       <c r="G549" s="3"/>
       <c r="H549" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="550" customHeight="1" ht="37.5" customFormat="1" s="8">
+    <row x14ac:dyDescent="0.25" r="550" customHeight="1" ht="37.5" customFormat="1" s="6">
       <c r="A550" s="2" t="s">
         <v>1383</v>
       </c>
@@ -39196,7 +39291,7 @@
       <c r="A557" s="1" t="s">
         <v>1400</v>
       </c>
-      <c r="B557" s="10" t="s">
+      <c r="B557" s="8" t="s">
         <v>1401</v>
       </c>
       <c r="C557" s="1" t="s">
@@ -39212,7 +39307,7 @@
       <c r="A558" s="1" t="s">
         <v>1403</v>
       </c>
-      <c r="B558" s="10" t="s">
+      <c r="B558" s="8" t="s">
         <v>1404</v>
       </c>
       <c r="C558" s="1" t="s">
@@ -40983,11 +41078,11 @@
       <c r="H675" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="676" customHeight="1" ht="19.5">
-      <c r="A676" s="6"/>
-      <c r="B676" s="6"/>
-      <c r="C676" s="6"/>
-      <c r="D676" s="7"/>
-      <c r="E676" s="7"/>
+      <c r="A676" s="1"/>
+      <c r="B676" s="1"/>
+      <c r="C676" s="1"/>
+      <c r="D676" s="2"/>
+      <c r="E676" s="2"/>
       <c r="F676" s="3"/>
       <c r="G676" s="3"/>
       <c r="H676" s="3"/>
@@ -46337,51 +46432,51 @@
       <c r="H1020" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1021" customHeight="1" ht="19.5">
-      <c r="A1021" s="6"/>
-      <c r="B1021" s="6"/>
-      <c r="C1021" s="6"/>
-      <c r="D1021" s="7"/>
-      <c r="E1021" s="7"/>
+      <c r="A1021" s="1"/>
+      <c r="B1021" s="1"/>
+      <c r="C1021" s="1"/>
+      <c r="D1021" s="2"/>
+      <c r="E1021" s="2"/>
       <c r="F1021" s="3"/>
       <c r="G1021" s="3"/>
       <c r="H1021" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1022" customHeight="1" ht="19.5">
-      <c r="A1022" s="6"/>
-      <c r="B1022" s="6"/>
-      <c r="C1022" s="6"/>
-      <c r="D1022" s="7"/>
-      <c r="E1022" s="7"/>
+      <c r="A1022" s="1"/>
+      <c r="B1022" s="1"/>
+      <c r="C1022" s="1"/>
+      <c r="D1022" s="2"/>
+      <c r="E1022" s="2"/>
       <c r="F1022" s="3"/>
       <c r="G1022" s="3"/>
       <c r="H1022" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1023" customHeight="1" ht="19.5">
-      <c r="A1023" s="6"/>
-      <c r="B1023" s="6"/>
-      <c r="C1023" s="6"/>
-      <c r="D1023" s="7"/>
-      <c r="E1023" s="7"/>
+      <c r="A1023" s="1"/>
+      <c r="B1023" s="1"/>
+      <c r="C1023" s="1"/>
+      <c r="D1023" s="2"/>
+      <c r="E1023" s="2"/>
       <c r="F1023" s="3"/>
       <c r="G1023" s="3"/>
       <c r="H1023" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1024" customHeight="1" ht="19.5">
-      <c r="A1024" s="6"/>
-      <c r="B1024" s="6"/>
-      <c r="C1024" s="6"/>
-      <c r="D1024" s="7"/>
-      <c r="E1024" s="7"/>
+      <c r="A1024" s="1"/>
+      <c r="B1024" s="1"/>
+      <c r="C1024" s="1"/>
+      <c r="D1024" s="2"/>
+      <c r="E1024" s="2"/>
       <c r="F1024" s="3"/>
       <c r="G1024" s="3"/>
       <c r="H1024" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1025" customHeight="1" ht="19.5">
-      <c r="A1025" s="6"/>
-      <c r="B1025" s="6"/>
-      <c r="C1025" s="6"/>
-      <c r="D1025" s="7"/>
-      <c r="E1025" s="7"/>
+      <c r="A1025" s="1"/>
+      <c r="B1025" s="1"/>
+      <c r="C1025" s="1"/>
+      <c r="D1025" s="2"/>
+      <c r="E1025" s="2"/>
       <c r="F1025" s="3"/>
       <c r="G1025" s="3"/>
       <c r="H1025" s="3"/>
@@ -47971,21 +48066,21 @@
       <c r="H1124" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1125" customHeight="1" ht="19.5">
-      <c r="A1125" s="6"/>
-      <c r="B1125" s="6"/>
-      <c r="C1125" s="6"/>
-      <c r="D1125" s="7"/>
-      <c r="E1125" s="7"/>
+      <c r="A1125" s="1"/>
+      <c r="B1125" s="1"/>
+      <c r="C1125" s="1"/>
+      <c r="D1125" s="2"/>
+      <c r="E1125" s="2"/>
       <c r="F1125" s="3"/>
       <c r="G1125" s="3"/>
       <c r="H1125" s="3"/>
     </row>
     <row x14ac:dyDescent="0.25" r="1126" customHeight="1" ht="19.5">
-      <c r="A1126" s="6"/>
-      <c r="B1126" s="6"/>
-      <c r="C1126" s="6"/>
-      <c r="D1126" s="7"/>
-      <c r="E1126" s="7"/>
+      <c r="A1126" s="1"/>
+      <c r="B1126" s="1"/>
+      <c r="C1126" s="1"/>
+      <c r="D1126" s="2"/>
+      <c r="E1126" s="2"/>
       <c r="F1126" s="3"/>
       <c r="G1126" s="3"/>
       <c r="H1126" s="3"/>

</xml_diff>